<commit_message>
Added Pause screen state check.  Also checks for Heart/Boo during pause screen
</commit_message>
<xml_diff>
--- a/MM2LogTemplate.xlsx
+++ b/MM2LogTemplate.xlsx
@@ -11,22 +11,26 @@
     <definedName name="Deaths">Sheet1!$E$3:$E$501</definedName>
     <definedName name="Hearts">Sheet1!$D$3:$D$501</definedName>
     <definedName name="Codes">Sheet1!$A$3:$A$501</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$2:$G$4</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_AADD0144_9195_49E4_9822_F67AE472B802_.wvu.FilterData">Sheet1!$B$7</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DAF9E434_143D_4C2F_BD3A_F42958B886A7_.wvu.FilterData">Sheet1!$A$3:$A$28</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_3557EC7E_8B9C_4DD1_84AC_D25832B36FAD_.wvu.FilterData">Sheet1!$A$4:$A$501</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$2:$I$4</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_F420EFAA_E1E7_4C15_A18B_9F49B707E26E_.wvu.FilterData">Sheet1!$A$4:$A$501</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_1D7BF479_05B9_4152_9B2B_CFBDDFCD1068_.wvu.FilterData">Sheet1!$A$2:$G$4</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4318B231_53B8_4726_82BD_03FDEDD286E4_.wvu.FilterData">Sheet1!$A$3:$A$28</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_AFAA05CB_82C0_46F8_B97B_1146D381C75C_.wvu.FilterData">Sheet1!$A$2:$G$4</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B936B0B1_DF02_40D5_BCB6_86CF286B23A4_.wvu.FilterData">Sheet1!$B$7</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DAF9E434-143D-4C2F-BD3A-F42958B886A7}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AADD0144-9195-49E4-9822-F67AE472B802}" name="Filter 3"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3557EC7E-8B9C-4DD1-84AC-D25832B36FAD}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AFAA05CB-82C0-46F8-B97B-1146D381C75C}" name="Filter 4"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1D7BF479-05B9-4152-9B2B-CFBDDFCD1068}" name="Filter 5"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4318B231-53B8-4726-82BD-03FDEDD286E4}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B936B0B1-DF02-40D5-BCB6-86CF286B23A4}" name="Filter 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F420EFAA-E1E7-4C15-A18B-9F49B707E26E}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MM2 Buddy Log</t>
   </si>
@@ -52,28 +56,10 @@
     <t>First Played</t>
   </si>
   <si>
-    <t>56G-JMK-KFF</t>
+    <t>Clear Time</t>
   </si>
   <si>
-    <t>Zeppelin Zapp</t>
-  </si>
-  <si>
-    <t>Traphic</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>5/3/2023 1949</t>
-  </si>
-  <si>
-    <t>M6J-H0N-PYG</t>
-  </si>
-  <si>
-    <t>Demon Desert</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>Translation</t>
   </si>
 </sst>
 </file>
@@ -128,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -147,13 +133,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -385,6 +365,8 @@
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -408,3050 +390,3029 @@
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="3">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5">
-      <c r="F5" s="9"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6">
-      <c r="F6" s="9"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7">
-      <c r="F7" s="9"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8">
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9">
-      <c r="F9" s="9"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10">
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11">
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12">
-      <c r="F12" s="9"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13">
-      <c r="F13" s="9"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14">
-      <c r="F14" s="9"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15">
-      <c r="F15" s="9"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16">
-      <c r="F16" s="9"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17">
-      <c r="F17" s="9"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18">
-      <c r="F18" s="9"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19">
-      <c r="F19" s="9"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20">
-      <c r="F20" s="9"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21">
-      <c r="F21" s="9"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22">
-      <c r="F22" s="9"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23">
-      <c r="F23" s="9"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24">
-      <c r="F24" s="9"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25">
-      <c r="F25" s="9"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26">
-      <c r="F26" s="9"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27">
-      <c r="F27" s="9"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28">
-      <c r="F28" s="9"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29">
-      <c r="F29" s="9"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30">
-      <c r="F30" s="9"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31">
-      <c r="F31" s="9"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32">
-      <c r="F32" s="9"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33">
-      <c r="F33" s="9"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34">
-      <c r="F34" s="9"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35">
-      <c r="F35" s="9"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36">
-      <c r="F36" s="9"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37">
-      <c r="F37" s="9"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38">
-      <c r="F38" s="9"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39">
-      <c r="F39" s="9"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40">
-      <c r="F40" s="9"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41">
-      <c r="F41" s="9"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42">
-      <c r="F42" s="9"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43">
-      <c r="F43" s="9"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44">
-      <c r="F44" s="9"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45">
-      <c r="F45" s="9"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46">
-      <c r="F46" s="9"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47">
-      <c r="F47" s="9"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48">
-      <c r="F48" s="9"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49">
-      <c r="F49" s="9"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50">
-      <c r="F50" s="9"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51">
-      <c r="F51" s="9"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52">
-      <c r="F52" s="9"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53">
-      <c r="F53" s="9"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54">
-      <c r="F54" s="9"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55">
-      <c r="F55" s="9"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56">
-      <c r="F56" s="9"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="57">
-      <c r="F57" s="9"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58">
-      <c r="F58" s="9"/>
+      <c r="F58" s="7"/>
     </row>
     <row r="59">
-      <c r="F59" s="9"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60">
-      <c r="F60" s="9"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61">
-      <c r="F61" s="9"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62">
-      <c r="F62" s="9"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="63">
-      <c r="F63" s="9"/>
+      <c r="F63" s="7"/>
     </row>
     <row r="64">
-      <c r="F64" s="9"/>
+      <c r="F64" s="7"/>
     </row>
     <row r="65">
-      <c r="F65" s="9"/>
+      <c r="F65" s="7"/>
     </row>
     <row r="66">
-      <c r="F66" s="9"/>
+      <c r="F66" s="7"/>
     </row>
     <row r="67">
-      <c r="F67" s="9"/>
+      <c r="F67" s="7"/>
     </row>
     <row r="68">
-      <c r="F68" s="9"/>
+      <c r="F68" s="7"/>
     </row>
     <row r="69">
-      <c r="F69" s="9"/>
+      <c r="F69" s="7"/>
     </row>
     <row r="70">
-      <c r="F70" s="9"/>
+      <c r="F70" s="7"/>
     </row>
     <row r="71">
-      <c r="F71" s="9"/>
+      <c r="F71" s="7"/>
     </row>
     <row r="72">
-      <c r="F72" s="9"/>
+      <c r="F72" s="7"/>
     </row>
     <row r="73">
-      <c r="F73" s="9"/>
+      <c r="F73" s="7"/>
     </row>
     <row r="74">
-      <c r="F74" s="9"/>
+      <c r="F74" s="7"/>
     </row>
     <row r="75">
-      <c r="F75" s="9"/>
+      <c r="F75" s="7"/>
     </row>
     <row r="76">
-      <c r="F76" s="9"/>
+      <c r="F76" s="7"/>
     </row>
     <row r="77">
-      <c r="F77" s="9"/>
+      <c r="F77" s="7"/>
     </row>
     <row r="78">
-      <c r="F78" s="9"/>
+      <c r="F78" s="7"/>
     </row>
     <row r="79">
-      <c r="F79" s="9"/>
+      <c r="F79" s="7"/>
     </row>
     <row r="80">
-      <c r="F80" s="9"/>
+      <c r="F80" s="7"/>
     </row>
     <row r="81">
-      <c r="F81" s="9"/>
+      <c r="F81" s="7"/>
     </row>
     <row r="82">
-      <c r="F82" s="9"/>
+      <c r="F82" s="7"/>
     </row>
     <row r="83">
-      <c r="F83" s="9"/>
+      <c r="F83" s="7"/>
     </row>
     <row r="84">
-      <c r="F84" s="9"/>
+      <c r="F84" s="7"/>
     </row>
     <row r="85">
-      <c r="F85" s="9"/>
+      <c r="F85" s="7"/>
     </row>
     <row r="86">
-      <c r="F86" s="9"/>
+      <c r="F86" s="7"/>
     </row>
     <row r="87">
-      <c r="F87" s="9"/>
+      <c r="F87" s="7"/>
     </row>
     <row r="88">
-      <c r="F88" s="9"/>
+      <c r="F88" s="7"/>
     </row>
     <row r="89">
-      <c r="F89" s="9"/>
+      <c r="F89" s="7"/>
     </row>
     <row r="90">
-      <c r="F90" s="9"/>
+      <c r="F90" s="7"/>
     </row>
     <row r="91">
-      <c r="F91" s="9"/>
+      <c r="F91" s="7"/>
     </row>
     <row r="92">
-      <c r="F92" s="9"/>
+      <c r="F92" s="7"/>
     </row>
     <row r="93">
-      <c r="F93" s="9"/>
+      <c r="F93" s="7"/>
     </row>
     <row r="94">
-      <c r="F94" s="9"/>
+      <c r="F94" s="7"/>
     </row>
     <row r="95">
-      <c r="F95" s="9"/>
+      <c r="F95" s="7"/>
     </row>
     <row r="96">
-      <c r="F96" s="9"/>
+      <c r="F96" s="7"/>
     </row>
     <row r="97">
-      <c r="F97" s="9"/>
+      <c r="F97" s="7"/>
     </row>
     <row r="98">
-      <c r="F98" s="9"/>
+      <c r="F98" s="7"/>
     </row>
     <row r="99">
-      <c r="F99" s="9"/>
+      <c r="F99" s="7"/>
     </row>
     <row r="100">
-      <c r="F100" s="9"/>
+      <c r="F100" s="7"/>
     </row>
     <row r="101">
-      <c r="F101" s="9"/>
+      <c r="F101" s="7"/>
     </row>
     <row r="102">
-      <c r="F102" s="9"/>
+      <c r="F102" s="7"/>
     </row>
     <row r="103">
-      <c r="F103" s="9"/>
+      <c r="F103" s="7"/>
     </row>
     <row r="104">
-      <c r="F104" s="9"/>
+      <c r="F104" s="7"/>
     </row>
     <row r="105">
-      <c r="F105" s="9"/>
+      <c r="F105" s="7"/>
     </row>
     <row r="106">
-      <c r="F106" s="9"/>
+      <c r="F106" s="7"/>
     </row>
     <row r="107">
-      <c r="F107" s="9"/>
+      <c r="F107" s="7"/>
     </row>
     <row r="108">
-      <c r="F108" s="9"/>
+      <c r="F108" s="7"/>
     </row>
     <row r="109">
-      <c r="F109" s="9"/>
+      <c r="F109" s="7"/>
     </row>
     <row r="110">
-      <c r="F110" s="9"/>
+      <c r="F110" s="7"/>
     </row>
     <row r="111">
-      <c r="F111" s="9"/>
+      <c r="F111" s="7"/>
     </row>
     <row r="112">
-      <c r="F112" s="9"/>
+      <c r="F112" s="7"/>
     </row>
     <row r="113">
-      <c r="F113" s="9"/>
+      <c r="F113" s="7"/>
     </row>
     <row r="114">
-      <c r="F114" s="9"/>
+      <c r="F114" s="7"/>
     </row>
     <row r="115">
-      <c r="F115" s="9"/>
+      <c r="F115" s="7"/>
     </row>
     <row r="116">
-      <c r="F116" s="9"/>
+      <c r="F116" s="7"/>
     </row>
     <row r="117">
-      <c r="F117" s="9"/>
+      <c r="F117" s="7"/>
     </row>
     <row r="118">
-      <c r="F118" s="9"/>
+      <c r="F118" s="7"/>
     </row>
     <row r="119">
-      <c r="F119" s="9"/>
+      <c r="F119" s="7"/>
     </row>
     <row r="120">
-      <c r="F120" s="9"/>
+      <c r="F120" s="7"/>
     </row>
     <row r="121">
-      <c r="F121" s="9"/>
+      <c r="F121" s="7"/>
     </row>
     <row r="122">
-      <c r="F122" s="9"/>
+      <c r="F122" s="7"/>
     </row>
     <row r="123">
-      <c r="F123" s="9"/>
+      <c r="F123" s="7"/>
     </row>
     <row r="124">
-      <c r="F124" s="9"/>
+      <c r="F124" s="7"/>
     </row>
     <row r="125">
-      <c r="F125" s="9"/>
+      <c r="F125" s="7"/>
     </row>
     <row r="126">
-      <c r="F126" s="9"/>
+      <c r="F126" s="7"/>
     </row>
     <row r="127">
-      <c r="F127" s="9"/>
+      <c r="F127" s="7"/>
     </row>
     <row r="128">
-      <c r="F128" s="9"/>
+      <c r="F128" s="7"/>
     </row>
     <row r="129">
-      <c r="F129" s="9"/>
+      <c r="F129" s="7"/>
     </row>
     <row r="130">
-      <c r="F130" s="9"/>
+      <c r="F130" s="7"/>
     </row>
     <row r="131">
-      <c r="F131" s="9"/>
+      <c r="F131" s="7"/>
     </row>
     <row r="132">
-      <c r="F132" s="9"/>
+      <c r="F132" s="7"/>
     </row>
     <row r="133">
-      <c r="F133" s="9"/>
+      <c r="F133" s="7"/>
     </row>
     <row r="134">
-      <c r="F134" s="9"/>
+      <c r="F134" s="7"/>
     </row>
     <row r="135">
-      <c r="F135" s="9"/>
+      <c r="F135" s="7"/>
     </row>
     <row r="136">
-      <c r="F136" s="9"/>
+      <c r="F136" s="7"/>
     </row>
     <row r="137">
-      <c r="F137" s="9"/>
+      <c r="F137" s="7"/>
     </row>
     <row r="138">
-      <c r="F138" s="9"/>
+      <c r="F138" s="7"/>
     </row>
     <row r="139">
-      <c r="F139" s="9"/>
+      <c r="F139" s="7"/>
     </row>
     <row r="140">
-      <c r="F140" s="9"/>
+      <c r="F140" s="7"/>
     </row>
     <row r="141">
-      <c r="F141" s="9"/>
+      <c r="F141" s="7"/>
     </row>
     <row r="142">
-      <c r="F142" s="9"/>
+      <c r="F142" s="7"/>
     </row>
     <row r="143">
-      <c r="F143" s="9"/>
+      <c r="F143" s="7"/>
     </row>
     <row r="144">
-      <c r="F144" s="9"/>
+      <c r="F144" s="7"/>
     </row>
     <row r="145">
-      <c r="F145" s="9"/>
+      <c r="F145" s="7"/>
     </row>
     <row r="146">
-      <c r="F146" s="9"/>
+      <c r="F146" s="7"/>
     </row>
     <row r="147">
-      <c r="F147" s="9"/>
+      <c r="F147" s="7"/>
     </row>
     <row r="148">
-      <c r="F148" s="9"/>
+      <c r="F148" s="7"/>
     </row>
     <row r="149">
-      <c r="F149" s="9"/>
+      <c r="F149" s="7"/>
     </row>
     <row r="150">
-      <c r="F150" s="9"/>
+      <c r="F150" s="7"/>
     </row>
     <row r="151">
-      <c r="F151" s="9"/>
+      <c r="F151" s="7"/>
     </row>
     <row r="152">
-      <c r="F152" s="9"/>
+      <c r="F152" s="7"/>
     </row>
     <row r="153">
-      <c r="F153" s="9"/>
+      <c r="F153" s="7"/>
     </row>
     <row r="154">
-      <c r="F154" s="9"/>
+      <c r="F154" s="7"/>
     </row>
     <row r="155">
-      <c r="F155" s="9"/>
+      <c r="F155" s="7"/>
     </row>
     <row r="156">
-      <c r="F156" s="9"/>
+      <c r="F156" s="7"/>
     </row>
     <row r="157">
-      <c r="F157" s="9"/>
+      <c r="F157" s="7"/>
     </row>
     <row r="158">
-      <c r="F158" s="9"/>
+      <c r="F158" s="7"/>
     </row>
     <row r="159">
-      <c r="F159" s="9"/>
+      <c r="F159" s="7"/>
     </row>
     <row r="160">
-      <c r="F160" s="9"/>
+      <c r="F160" s="7"/>
     </row>
     <row r="161">
-      <c r="F161" s="9"/>
+      <c r="F161" s="7"/>
     </row>
     <row r="162">
-      <c r="F162" s="9"/>
+      <c r="F162" s="7"/>
     </row>
     <row r="163">
-      <c r="F163" s="9"/>
+      <c r="F163" s="7"/>
     </row>
     <row r="164">
-      <c r="F164" s="9"/>
+      <c r="F164" s="7"/>
     </row>
     <row r="165">
-      <c r="F165" s="9"/>
+      <c r="F165" s="7"/>
     </row>
     <row r="166">
-      <c r="F166" s="9"/>
+      <c r="F166" s="7"/>
     </row>
     <row r="167">
-      <c r="F167" s="9"/>
+      <c r="F167" s="7"/>
     </row>
     <row r="168">
-      <c r="F168" s="9"/>
+      <c r="F168" s="7"/>
     </row>
     <row r="169">
-      <c r="F169" s="9"/>
+      <c r="F169" s="7"/>
     </row>
     <row r="170">
-      <c r="F170" s="9"/>
+      <c r="F170" s="7"/>
     </row>
     <row r="171">
-      <c r="F171" s="9"/>
+      <c r="F171" s="7"/>
     </row>
     <row r="172">
-      <c r="F172" s="9"/>
+      <c r="F172" s="7"/>
     </row>
     <row r="173">
-      <c r="F173" s="9"/>
+      <c r="F173" s="7"/>
     </row>
     <row r="174">
-      <c r="F174" s="9"/>
+      <c r="F174" s="7"/>
     </row>
     <row r="175">
-      <c r="F175" s="9"/>
+      <c r="F175" s="7"/>
     </row>
     <row r="176">
-      <c r="F176" s="9"/>
+      <c r="F176" s="7"/>
     </row>
     <row r="177">
-      <c r="F177" s="9"/>
+      <c r="F177" s="7"/>
     </row>
     <row r="178">
-      <c r="F178" s="9"/>
+      <c r="F178" s="7"/>
     </row>
     <row r="179">
-      <c r="F179" s="9"/>
+      <c r="F179" s="7"/>
     </row>
     <row r="180">
-      <c r="F180" s="9"/>
+      <c r="F180" s="7"/>
     </row>
     <row r="181">
-      <c r="F181" s="9"/>
+      <c r="F181" s="7"/>
     </row>
     <row r="182">
-      <c r="F182" s="9"/>
+      <c r="F182" s="7"/>
     </row>
     <row r="183">
-      <c r="F183" s="9"/>
+      <c r="F183" s="7"/>
     </row>
     <row r="184">
-      <c r="F184" s="9"/>
+      <c r="F184" s="7"/>
     </row>
     <row r="185">
-      <c r="F185" s="9"/>
+      <c r="F185" s="7"/>
     </row>
     <row r="186">
-      <c r="F186" s="9"/>
+      <c r="F186" s="7"/>
     </row>
     <row r="187">
-      <c r="F187" s="9"/>
+      <c r="F187" s="7"/>
     </row>
     <row r="188">
-      <c r="F188" s="9"/>
+      <c r="F188" s="7"/>
     </row>
     <row r="189">
-      <c r="F189" s="9"/>
+      <c r="F189" s="7"/>
     </row>
     <row r="190">
-      <c r="F190" s="9"/>
+      <c r="F190" s="7"/>
     </row>
     <row r="191">
-      <c r="F191" s="9"/>
+      <c r="F191" s="7"/>
     </row>
     <row r="192">
-      <c r="F192" s="9"/>
+      <c r="F192" s="7"/>
     </row>
     <row r="193">
-      <c r="F193" s="9"/>
+      <c r="F193" s="7"/>
     </row>
     <row r="194">
-      <c r="F194" s="9"/>
+      <c r="F194" s="7"/>
     </row>
     <row r="195">
-      <c r="F195" s="9"/>
+      <c r="F195" s="7"/>
     </row>
     <row r="196">
-      <c r="F196" s="9"/>
+      <c r="F196" s="7"/>
     </row>
     <row r="197">
-      <c r="F197" s="9"/>
+      <c r="F197" s="7"/>
     </row>
     <row r="198">
-      <c r="F198" s="9"/>
+      <c r="F198" s="7"/>
     </row>
     <row r="199">
-      <c r="F199" s="9"/>
+      <c r="F199" s="7"/>
     </row>
     <row r="200">
-      <c r="F200" s="9"/>
+      <c r="F200" s="7"/>
     </row>
     <row r="201">
-      <c r="F201" s="9"/>
+      <c r="F201" s="7"/>
     </row>
     <row r="202">
-      <c r="F202" s="9"/>
+      <c r="F202" s="7"/>
     </row>
     <row r="203">
-      <c r="F203" s="9"/>
+      <c r="F203" s="7"/>
     </row>
     <row r="204">
-      <c r="F204" s="9"/>
+      <c r="F204" s="7"/>
     </row>
     <row r="205">
-      <c r="F205" s="9"/>
+      <c r="F205" s="7"/>
     </row>
     <row r="206">
-      <c r="F206" s="9"/>
+      <c r="F206" s="7"/>
     </row>
     <row r="207">
-      <c r="F207" s="9"/>
+      <c r="F207" s="7"/>
     </row>
     <row r="208">
-      <c r="F208" s="9"/>
+      <c r="F208" s="7"/>
     </row>
     <row r="209">
-      <c r="F209" s="9"/>
+      <c r="F209" s="7"/>
     </row>
     <row r="210">
-      <c r="F210" s="9"/>
+      <c r="F210" s="7"/>
     </row>
     <row r="211">
-      <c r="F211" s="9"/>
+      <c r="F211" s="7"/>
     </row>
     <row r="212">
-      <c r="F212" s="9"/>
+      <c r="F212" s="7"/>
     </row>
     <row r="213">
-      <c r="F213" s="9"/>
+      <c r="F213" s="7"/>
     </row>
     <row r="214">
-      <c r="F214" s="9"/>
+      <c r="F214" s="7"/>
     </row>
     <row r="215">
-      <c r="F215" s="9"/>
+      <c r="F215" s="7"/>
     </row>
     <row r="216">
-      <c r="F216" s="9"/>
+      <c r="F216" s="7"/>
     </row>
     <row r="217">
-      <c r="F217" s="9"/>
+      <c r="F217" s="7"/>
     </row>
     <row r="218">
-      <c r="F218" s="9"/>
+      <c r="F218" s="7"/>
     </row>
     <row r="219">
-      <c r="F219" s="9"/>
+      <c r="F219" s="7"/>
     </row>
     <row r="220">
-      <c r="F220" s="9"/>
+      <c r="F220" s="7"/>
     </row>
     <row r="221">
-      <c r="F221" s="9"/>
+      <c r="F221" s="7"/>
     </row>
     <row r="222">
-      <c r="F222" s="9"/>
+      <c r="F222" s="7"/>
     </row>
     <row r="223">
-      <c r="F223" s="9"/>
+      <c r="F223" s="7"/>
     </row>
     <row r="224">
-      <c r="F224" s="9"/>
+      <c r="F224" s="7"/>
     </row>
     <row r="225">
-      <c r="F225" s="9"/>
+      <c r="F225" s="7"/>
     </row>
     <row r="226">
-      <c r="F226" s="9"/>
+      <c r="F226" s="7"/>
     </row>
     <row r="227">
-      <c r="F227" s="9"/>
+      <c r="F227" s="7"/>
     </row>
     <row r="228">
-      <c r="F228" s="9"/>
+      <c r="F228" s="7"/>
     </row>
     <row r="229">
-      <c r="F229" s="9"/>
+      <c r="F229" s="7"/>
     </row>
     <row r="230">
-      <c r="F230" s="9"/>
+      <c r="F230" s="7"/>
     </row>
     <row r="231">
-      <c r="F231" s="9"/>
+      <c r="F231" s="7"/>
     </row>
     <row r="232">
-      <c r="F232" s="9"/>
+      <c r="F232" s="7"/>
     </row>
     <row r="233">
-      <c r="F233" s="9"/>
+      <c r="F233" s="7"/>
     </row>
     <row r="234">
-      <c r="F234" s="9"/>
+      <c r="F234" s="7"/>
     </row>
     <row r="235">
-      <c r="F235" s="9"/>
+      <c r="F235" s="7"/>
     </row>
     <row r="236">
-      <c r="F236" s="9"/>
+      <c r="F236" s="7"/>
     </row>
     <row r="237">
-      <c r="F237" s="9"/>
+      <c r="F237" s="7"/>
     </row>
     <row r="238">
-      <c r="F238" s="9"/>
+      <c r="F238" s="7"/>
     </row>
     <row r="239">
-      <c r="F239" s="9"/>
+      <c r="F239" s="7"/>
     </row>
     <row r="240">
-      <c r="F240" s="9"/>
+      <c r="F240" s="7"/>
     </row>
     <row r="241">
-      <c r="F241" s="9"/>
+      <c r="F241" s="7"/>
     </row>
     <row r="242">
-      <c r="F242" s="9"/>
+      <c r="F242" s="7"/>
     </row>
     <row r="243">
-      <c r="F243" s="9"/>
+      <c r="F243" s="7"/>
     </row>
     <row r="244">
-      <c r="F244" s="9"/>
+      <c r="F244" s="7"/>
     </row>
     <row r="245">
-      <c r="F245" s="9"/>
+      <c r="F245" s="7"/>
     </row>
     <row r="246">
-      <c r="F246" s="9"/>
+      <c r="F246" s="7"/>
     </row>
     <row r="247">
-      <c r="F247" s="9"/>
+      <c r="F247" s="7"/>
     </row>
     <row r="248">
-      <c r="F248" s="9"/>
+      <c r="F248" s="7"/>
     </row>
     <row r="249">
-      <c r="F249" s="9"/>
+      <c r="F249" s="7"/>
     </row>
     <row r="250">
-      <c r="F250" s="9"/>
+      <c r="F250" s="7"/>
     </row>
     <row r="251">
-      <c r="F251" s="9"/>
+      <c r="F251" s="7"/>
     </row>
     <row r="252">
-      <c r="F252" s="9"/>
+      <c r="F252" s="7"/>
     </row>
     <row r="253">
-      <c r="F253" s="9"/>
+      <c r="F253" s="7"/>
     </row>
     <row r="254">
-      <c r="F254" s="9"/>
+      <c r="F254" s="7"/>
     </row>
     <row r="255">
-      <c r="F255" s="9"/>
+      <c r="F255" s="7"/>
     </row>
     <row r="256">
-      <c r="F256" s="9"/>
+      <c r="F256" s="7"/>
     </row>
     <row r="257">
-      <c r="F257" s="9"/>
+      <c r="F257" s="7"/>
     </row>
     <row r="258">
-      <c r="F258" s="9"/>
+      <c r="F258" s="7"/>
     </row>
     <row r="259">
-      <c r="F259" s="9"/>
+      <c r="F259" s="7"/>
     </row>
     <row r="260">
-      <c r="F260" s="9"/>
+      <c r="F260" s="7"/>
     </row>
     <row r="261">
-      <c r="F261" s="9"/>
+      <c r="F261" s="7"/>
     </row>
     <row r="262">
-      <c r="F262" s="9"/>
+      <c r="F262" s="7"/>
     </row>
     <row r="263">
-      <c r="F263" s="9"/>
+      <c r="F263" s="7"/>
     </row>
     <row r="264">
-      <c r="F264" s="9"/>
+      <c r="F264" s="7"/>
     </row>
     <row r="265">
-      <c r="F265" s="9"/>
+      <c r="F265" s="7"/>
     </row>
     <row r="266">
-      <c r="F266" s="9"/>
+      <c r="F266" s="7"/>
     </row>
     <row r="267">
-      <c r="F267" s="9"/>
+      <c r="F267" s="7"/>
     </row>
     <row r="268">
-      <c r="F268" s="9"/>
+      <c r="F268" s="7"/>
     </row>
     <row r="269">
-      <c r="F269" s="9"/>
+      <c r="F269" s="7"/>
     </row>
     <row r="270">
-      <c r="F270" s="9"/>
+      <c r="F270" s="7"/>
     </row>
     <row r="271">
-      <c r="F271" s="9"/>
+      <c r="F271" s="7"/>
     </row>
     <row r="272">
-      <c r="F272" s="9"/>
+      <c r="F272" s="7"/>
     </row>
     <row r="273">
-      <c r="F273" s="9"/>
+      <c r="F273" s="7"/>
     </row>
     <row r="274">
-      <c r="F274" s="9"/>
+      <c r="F274" s="7"/>
     </row>
     <row r="275">
-      <c r="F275" s="9"/>
+      <c r="F275" s="7"/>
     </row>
     <row r="276">
-      <c r="F276" s="9"/>
+      <c r="F276" s="7"/>
     </row>
     <row r="277">
-      <c r="F277" s="9"/>
+      <c r="F277" s="7"/>
     </row>
     <row r="278">
-      <c r="F278" s="9"/>
+      <c r="F278" s="7"/>
     </row>
     <row r="279">
-      <c r="F279" s="9"/>
+      <c r="F279" s="7"/>
     </row>
     <row r="280">
-      <c r="F280" s="9"/>
+      <c r="F280" s="7"/>
     </row>
     <row r="281">
-      <c r="F281" s="9"/>
+      <c r="F281" s="7"/>
     </row>
     <row r="282">
-      <c r="F282" s="9"/>
+      <c r="F282" s="7"/>
     </row>
     <row r="283">
-      <c r="F283" s="9"/>
+      <c r="F283" s="7"/>
     </row>
     <row r="284">
-      <c r="F284" s="9"/>
+      <c r="F284" s="7"/>
     </row>
     <row r="285">
-      <c r="F285" s="9"/>
+      <c r="F285" s="7"/>
     </row>
     <row r="286">
-      <c r="F286" s="9"/>
+      <c r="F286" s="7"/>
     </row>
     <row r="287">
-      <c r="F287" s="9"/>
+      <c r="F287" s="7"/>
     </row>
     <row r="288">
-      <c r="F288" s="9"/>
+      <c r="F288" s="7"/>
     </row>
     <row r="289">
-      <c r="F289" s="9"/>
+      <c r="F289" s="7"/>
     </row>
     <row r="290">
-      <c r="F290" s="9"/>
+      <c r="F290" s="7"/>
     </row>
     <row r="291">
-      <c r="F291" s="9"/>
+      <c r="F291" s="7"/>
     </row>
     <row r="292">
-      <c r="F292" s="9"/>
+      <c r="F292" s="7"/>
     </row>
     <row r="293">
-      <c r="F293" s="9"/>
+      <c r="F293" s="7"/>
     </row>
     <row r="294">
-      <c r="F294" s="9"/>
+      <c r="F294" s="7"/>
     </row>
     <row r="295">
-      <c r="F295" s="9"/>
+      <c r="F295" s="7"/>
     </row>
     <row r="296">
-      <c r="F296" s="9"/>
+      <c r="F296" s="7"/>
     </row>
     <row r="297">
-      <c r="F297" s="9"/>
+      <c r="F297" s="7"/>
     </row>
     <row r="298">
-      <c r="F298" s="9"/>
+      <c r="F298" s="7"/>
     </row>
     <row r="299">
-      <c r="F299" s="9"/>
+      <c r="F299" s="7"/>
     </row>
     <row r="300">
-      <c r="F300" s="9"/>
+      <c r="F300" s="7"/>
     </row>
     <row r="301">
-      <c r="F301" s="9"/>
+      <c r="F301" s="7"/>
     </row>
     <row r="302">
-      <c r="F302" s="9"/>
+      <c r="F302" s="7"/>
     </row>
     <row r="303">
-      <c r="F303" s="9"/>
+      <c r="F303" s="7"/>
     </row>
     <row r="304">
-      <c r="F304" s="9"/>
+      <c r="F304" s="7"/>
     </row>
     <row r="305">
-      <c r="F305" s="9"/>
+      <c r="F305" s="7"/>
     </row>
     <row r="306">
-      <c r="F306" s="9"/>
+      <c r="F306" s="7"/>
     </row>
     <row r="307">
-      <c r="F307" s="9"/>
+      <c r="F307" s="7"/>
     </row>
     <row r="308">
-      <c r="F308" s="9"/>
+      <c r="F308" s="7"/>
     </row>
     <row r="309">
-      <c r="F309" s="9"/>
+      <c r="F309" s="7"/>
     </row>
     <row r="310">
-      <c r="F310" s="9"/>
+      <c r="F310" s="7"/>
     </row>
     <row r="311">
-      <c r="F311" s="9"/>
+      <c r="F311" s="7"/>
     </row>
     <row r="312">
-      <c r="F312" s="9"/>
+      <c r="F312" s="7"/>
     </row>
     <row r="313">
-      <c r="F313" s="9"/>
+      <c r="F313" s="7"/>
     </row>
     <row r="314">
-      <c r="F314" s="9"/>
+      <c r="F314" s="7"/>
     </row>
     <row r="315">
-      <c r="F315" s="9"/>
+      <c r="F315" s="7"/>
     </row>
     <row r="316">
-      <c r="F316" s="9"/>
+      <c r="F316" s="7"/>
     </row>
     <row r="317">
-      <c r="F317" s="9"/>
+      <c r="F317" s="7"/>
     </row>
     <row r="318">
-      <c r="F318" s="9"/>
+      <c r="F318" s="7"/>
     </row>
     <row r="319">
-      <c r="F319" s="9"/>
+      <c r="F319" s="7"/>
     </row>
     <row r="320">
-      <c r="F320" s="9"/>
+      <c r="F320" s="7"/>
     </row>
     <row r="321">
-      <c r="F321" s="9"/>
+      <c r="F321" s="7"/>
     </row>
     <row r="322">
-      <c r="F322" s="9"/>
+      <c r="F322" s="7"/>
     </row>
     <row r="323">
-      <c r="F323" s="9"/>
+      <c r="F323" s="7"/>
     </row>
     <row r="324">
-      <c r="F324" s="9"/>
+      <c r="F324" s="7"/>
     </row>
     <row r="325">
-      <c r="F325" s="9"/>
+      <c r="F325" s="7"/>
     </row>
     <row r="326">
-      <c r="F326" s="9"/>
+      <c r="F326" s="7"/>
     </row>
     <row r="327">
-      <c r="F327" s="9"/>
+      <c r="F327" s="7"/>
     </row>
     <row r="328">
-      <c r="F328" s="9"/>
+      <c r="F328" s="7"/>
     </row>
     <row r="329">
-      <c r="F329" s="9"/>
+      <c r="F329" s="7"/>
     </row>
     <row r="330">
-      <c r="F330" s="9"/>
+      <c r="F330" s="7"/>
     </row>
     <row r="331">
-      <c r="F331" s="9"/>
+      <c r="F331" s="7"/>
     </row>
     <row r="332">
-      <c r="F332" s="9"/>
+      <c r="F332" s="7"/>
     </row>
     <row r="333">
-      <c r="F333" s="9"/>
+      <c r="F333" s="7"/>
     </row>
     <row r="334">
-      <c r="F334" s="9"/>
+      <c r="F334" s="7"/>
     </row>
     <row r="335">
-      <c r="F335" s="9"/>
+      <c r="F335" s="7"/>
     </row>
     <row r="336">
-      <c r="F336" s="9"/>
+      <c r="F336" s="7"/>
     </row>
     <row r="337">
-      <c r="F337" s="9"/>
+      <c r="F337" s="7"/>
     </row>
     <row r="338">
-      <c r="F338" s="9"/>
+      <c r="F338" s="7"/>
     </row>
     <row r="339">
-      <c r="F339" s="9"/>
+      <c r="F339" s="7"/>
     </row>
     <row r="340">
-      <c r="F340" s="9"/>
+      <c r="F340" s="7"/>
     </row>
     <row r="341">
-      <c r="F341" s="9"/>
+      <c r="F341" s="7"/>
     </row>
     <row r="342">
-      <c r="F342" s="9"/>
+      <c r="F342" s="7"/>
     </row>
     <row r="343">
-      <c r="F343" s="9"/>
+      <c r="F343" s="7"/>
     </row>
     <row r="344">
-      <c r="F344" s="9"/>
+      <c r="F344" s="7"/>
     </row>
     <row r="345">
-      <c r="F345" s="9"/>
+      <c r="F345" s="7"/>
     </row>
     <row r="346">
-      <c r="F346" s="9"/>
+      <c r="F346" s="7"/>
     </row>
     <row r="347">
-      <c r="F347" s="9"/>
+      <c r="F347" s="7"/>
     </row>
     <row r="348">
-      <c r="F348" s="9"/>
+      <c r="F348" s="7"/>
     </row>
     <row r="349">
-      <c r="F349" s="9"/>
+      <c r="F349" s="7"/>
     </row>
     <row r="350">
-      <c r="F350" s="9"/>
+      <c r="F350" s="7"/>
     </row>
     <row r="351">
-      <c r="F351" s="9"/>
+      <c r="F351" s="7"/>
     </row>
     <row r="352">
-      <c r="F352" s="9"/>
+      <c r="F352" s="7"/>
     </row>
     <row r="353">
-      <c r="F353" s="9"/>
+      <c r="F353" s="7"/>
     </row>
     <row r="354">
-      <c r="F354" s="9"/>
+      <c r="F354" s="7"/>
     </row>
     <row r="355">
-      <c r="F355" s="9"/>
+      <c r="F355" s="7"/>
     </row>
     <row r="356">
-      <c r="F356" s="9"/>
+      <c r="F356" s="7"/>
     </row>
     <row r="357">
-      <c r="F357" s="9"/>
+      <c r="F357" s="7"/>
     </row>
     <row r="358">
-      <c r="F358" s="9"/>
+      <c r="F358" s="7"/>
     </row>
     <row r="359">
-      <c r="F359" s="9"/>
+      <c r="F359" s="7"/>
     </row>
     <row r="360">
-      <c r="F360" s="9"/>
+      <c r="F360" s="7"/>
     </row>
     <row r="361">
-      <c r="F361" s="9"/>
+      <c r="F361" s="7"/>
     </row>
     <row r="362">
-      <c r="F362" s="9"/>
+      <c r="F362" s="7"/>
     </row>
     <row r="363">
-      <c r="F363" s="9"/>
+      <c r="F363" s="7"/>
     </row>
     <row r="364">
-      <c r="F364" s="9"/>
+      <c r="F364" s="7"/>
     </row>
     <row r="365">
-      <c r="F365" s="9"/>
+      <c r="F365" s="7"/>
     </row>
     <row r="366">
-      <c r="F366" s="9"/>
+      <c r="F366" s="7"/>
     </row>
     <row r="367">
-      <c r="F367" s="9"/>
+      <c r="F367" s="7"/>
     </row>
     <row r="368">
-      <c r="F368" s="9"/>
+      <c r="F368" s="7"/>
     </row>
     <row r="369">
-      <c r="F369" s="9"/>
+      <c r="F369" s="7"/>
     </row>
     <row r="370">
-      <c r="F370" s="9"/>
+      <c r="F370" s="7"/>
     </row>
     <row r="371">
-      <c r="F371" s="9"/>
+      <c r="F371" s="7"/>
     </row>
     <row r="372">
-      <c r="F372" s="9"/>
+      <c r="F372" s="7"/>
     </row>
     <row r="373">
-      <c r="F373" s="9"/>
+      <c r="F373" s="7"/>
     </row>
     <row r="374">
-      <c r="F374" s="9"/>
+      <c r="F374" s="7"/>
     </row>
     <row r="375">
-      <c r="F375" s="9"/>
+      <c r="F375" s="7"/>
     </row>
     <row r="376">
-      <c r="F376" s="9"/>
+      <c r="F376" s="7"/>
     </row>
     <row r="377">
-      <c r="F377" s="9"/>
+      <c r="F377" s="7"/>
     </row>
     <row r="378">
-      <c r="F378" s="9"/>
+      <c r="F378" s="7"/>
     </row>
     <row r="379">
-      <c r="F379" s="9"/>
+      <c r="F379" s="7"/>
     </row>
     <row r="380">
-      <c r="F380" s="9"/>
+      <c r="F380" s="7"/>
     </row>
     <row r="381">
-      <c r="F381" s="9"/>
+      <c r="F381" s="7"/>
     </row>
     <row r="382">
-      <c r="F382" s="9"/>
+      <c r="F382" s="7"/>
     </row>
     <row r="383">
-      <c r="F383" s="9"/>
+      <c r="F383" s="7"/>
     </row>
     <row r="384">
-      <c r="F384" s="9"/>
+      <c r="F384" s="7"/>
     </row>
     <row r="385">
-      <c r="F385" s="9"/>
+      <c r="F385" s="7"/>
     </row>
     <row r="386">
-      <c r="F386" s="9"/>
+      <c r="F386" s="7"/>
     </row>
     <row r="387">
-      <c r="F387" s="9"/>
+      <c r="F387" s="7"/>
     </row>
     <row r="388">
-      <c r="F388" s="9"/>
+      <c r="F388" s="7"/>
     </row>
     <row r="389">
-      <c r="F389" s="9"/>
+      <c r="F389" s="7"/>
     </row>
     <row r="390">
-      <c r="F390" s="9"/>
+      <c r="F390" s="7"/>
     </row>
     <row r="391">
-      <c r="F391" s="9"/>
+      <c r="F391" s="7"/>
     </row>
     <row r="392">
-      <c r="F392" s="9"/>
+      <c r="F392" s="7"/>
     </row>
     <row r="393">
-      <c r="F393" s="9"/>
+      <c r="F393" s="7"/>
     </row>
     <row r="394">
-      <c r="F394" s="9"/>
+      <c r="F394" s="7"/>
     </row>
     <row r="395">
-      <c r="F395" s="9"/>
+      <c r="F395" s="7"/>
     </row>
     <row r="396">
-      <c r="F396" s="9"/>
+      <c r="F396" s="7"/>
     </row>
     <row r="397">
-      <c r="F397" s="9"/>
+      <c r="F397" s="7"/>
     </row>
     <row r="398">
-      <c r="F398" s="9"/>
+      <c r="F398" s="7"/>
     </row>
     <row r="399">
-      <c r="F399" s="9"/>
+      <c r="F399" s="7"/>
     </row>
     <row r="400">
-      <c r="F400" s="9"/>
+      <c r="F400" s="7"/>
     </row>
     <row r="401">
-      <c r="F401" s="9"/>
+      <c r="F401" s="7"/>
     </row>
     <row r="402">
-      <c r="F402" s="9"/>
+      <c r="F402" s="7"/>
     </row>
     <row r="403">
-      <c r="F403" s="9"/>
+      <c r="F403" s="7"/>
     </row>
     <row r="404">
-      <c r="F404" s="9"/>
+      <c r="F404" s="7"/>
     </row>
     <row r="405">
-      <c r="F405" s="9"/>
+      <c r="F405" s="7"/>
     </row>
     <row r="406">
-      <c r="F406" s="9"/>
+      <c r="F406" s="7"/>
     </row>
     <row r="407">
-      <c r="F407" s="9"/>
+      <c r="F407" s="7"/>
     </row>
     <row r="408">
-      <c r="F408" s="9"/>
+      <c r="F408" s="7"/>
     </row>
     <row r="409">
-      <c r="F409" s="9"/>
+      <c r="F409" s="7"/>
     </row>
     <row r="410">
-      <c r="F410" s="9"/>
+      <c r="F410" s="7"/>
     </row>
     <row r="411">
-      <c r="F411" s="9"/>
+      <c r="F411" s="7"/>
     </row>
     <row r="412">
-      <c r="F412" s="9"/>
+      <c r="F412" s="7"/>
     </row>
     <row r="413">
-      <c r="F413" s="9"/>
+      <c r="F413" s="7"/>
     </row>
     <row r="414">
-      <c r="F414" s="9"/>
+      <c r="F414" s="7"/>
     </row>
     <row r="415">
-      <c r="F415" s="9"/>
+      <c r="F415" s="7"/>
     </row>
     <row r="416">
-      <c r="F416" s="9"/>
+      <c r="F416" s="7"/>
     </row>
     <row r="417">
-      <c r="F417" s="9"/>
+      <c r="F417" s="7"/>
     </row>
     <row r="418">
-      <c r="F418" s="9"/>
+      <c r="F418" s="7"/>
     </row>
     <row r="419">
-      <c r="F419" s="9"/>
+      <c r="F419" s="7"/>
     </row>
     <row r="420">
-      <c r="F420" s="9"/>
+      <c r="F420" s="7"/>
     </row>
     <row r="421">
-      <c r="F421" s="9"/>
+      <c r="F421" s="7"/>
     </row>
     <row r="422">
-      <c r="F422" s="9"/>
+      <c r="F422" s="7"/>
     </row>
     <row r="423">
-      <c r="F423" s="9"/>
+      <c r="F423" s="7"/>
     </row>
     <row r="424">
-      <c r="F424" s="9"/>
+      <c r="F424" s="7"/>
     </row>
     <row r="425">
-      <c r="F425" s="9"/>
+      <c r="F425" s="7"/>
     </row>
     <row r="426">
-      <c r="F426" s="9"/>
+      <c r="F426" s="7"/>
     </row>
     <row r="427">
-      <c r="F427" s="9"/>
+      <c r="F427" s="7"/>
     </row>
     <row r="428">
-      <c r="F428" s="9"/>
+      <c r="F428" s="7"/>
     </row>
     <row r="429">
-      <c r="F429" s="9"/>
+      <c r="F429" s="7"/>
     </row>
     <row r="430">
-      <c r="F430" s="9"/>
+      <c r="F430" s="7"/>
     </row>
     <row r="431">
-      <c r="F431" s="9"/>
+      <c r="F431" s="7"/>
     </row>
     <row r="432">
-      <c r="F432" s="9"/>
+      <c r="F432" s="7"/>
     </row>
     <row r="433">
-      <c r="F433" s="9"/>
+      <c r="F433" s="7"/>
     </row>
     <row r="434">
-      <c r="F434" s="9"/>
+      <c r="F434" s="7"/>
     </row>
     <row r="435">
-      <c r="F435" s="9"/>
+      <c r="F435" s="7"/>
     </row>
     <row r="436">
-      <c r="F436" s="9"/>
+      <c r="F436" s="7"/>
     </row>
     <row r="437">
-      <c r="F437" s="9"/>
+      <c r="F437" s="7"/>
     </row>
     <row r="438">
-      <c r="F438" s="9"/>
+      <c r="F438" s="7"/>
     </row>
     <row r="439">
-      <c r="F439" s="9"/>
+      <c r="F439" s="7"/>
     </row>
     <row r="440">
-      <c r="F440" s="9"/>
+      <c r="F440" s="7"/>
     </row>
     <row r="441">
-      <c r="F441" s="9"/>
+      <c r="F441" s="7"/>
     </row>
     <row r="442">
-      <c r="F442" s="9"/>
+      <c r="F442" s="7"/>
     </row>
     <row r="443">
-      <c r="F443" s="9"/>
+      <c r="F443" s="7"/>
     </row>
     <row r="444">
-      <c r="F444" s="9"/>
+      <c r="F444" s="7"/>
     </row>
     <row r="445">
-      <c r="F445" s="9"/>
+      <c r="F445" s="7"/>
     </row>
     <row r="446">
-      <c r="F446" s="9"/>
+      <c r="F446" s="7"/>
     </row>
     <row r="447">
-      <c r="F447" s="9"/>
+      <c r="F447" s="7"/>
     </row>
     <row r="448">
-      <c r="F448" s="9"/>
+      <c r="F448" s="7"/>
     </row>
     <row r="449">
-      <c r="F449" s="9"/>
+      <c r="F449" s="7"/>
     </row>
     <row r="450">
-      <c r="F450" s="9"/>
+      <c r="F450" s="7"/>
     </row>
     <row r="451">
-      <c r="F451" s="9"/>
+      <c r="F451" s="7"/>
     </row>
     <row r="452">
-      <c r="F452" s="9"/>
+      <c r="F452" s="7"/>
     </row>
     <row r="453">
-      <c r="F453" s="9"/>
+      <c r="F453" s="7"/>
     </row>
     <row r="454">
-      <c r="F454" s="9"/>
+      <c r="F454" s="7"/>
     </row>
     <row r="455">
-      <c r="F455" s="9"/>
+      <c r="F455" s="7"/>
     </row>
     <row r="456">
-      <c r="F456" s="9"/>
+      <c r="F456" s="7"/>
     </row>
     <row r="457">
-      <c r="F457" s="9"/>
+      <c r="F457" s="7"/>
     </row>
     <row r="458">
-      <c r="F458" s="9"/>
+      <c r="F458" s="7"/>
     </row>
     <row r="459">
-      <c r="F459" s="9"/>
+      <c r="F459" s="7"/>
     </row>
     <row r="460">
-      <c r="F460" s="9"/>
+      <c r="F460" s="7"/>
     </row>
     <row r="461">
-      <c r="F461" s="9"/>
+      <c r="F461" s="7"/>
     </row>
     <row r="462">
-      <c r="F462" s="9"/>
+      <c r="F462" s="7"/>
     </row>
     <row r="463">
-      <c r="F463" s="9"/>
+      <c r="F463" s="7"/>
     </row>
     <row r="464">
-      <c r="F464" s="9"/>
+      <c r="F464" s="7"/>
     </row>
     <row r="465">
-      <c r="F465" s="9"/>
+      <c r="F465" s="7"/>
     </row>
     <row r="466">
-      <c r="F466" s="9"/>
+      <c r="F466" s="7"/>
     </row>
     <row r="467">
-      <c r="F467" s="9"/>
+      <c r="F467" s="7"/>
     </row>
     <row r="468">
-      <c r="F468" s="9"/>
+      <c r="F468" s="7"/>
     </row>
     <row r="469">
-      <c r="F469" s="9"/>
+      <c r="F469" s="7"/>
     </row>
     <row r="470">
-      <c r="F470" s="9"/>
+      <c r="F470" s="7"/>
     </row>
     <row r="471">
-      <c r="F471" s="9"/>
+      <c r="F471" s="7"/>
     </row>
     <row r="472">
-      <c r="F472" s="9"/>
+      <c r="F472" s="7"/>
     </row>
     <row r="473">
-      <c r="F473" s="9"/>
+      <c r="F473" s="7"/>
     </row>
     <row r="474">
-      <c r="F474" s="9"/>
+      <c r="F474" s="7"/>
     </row>
     <row r="475">
-      <c r="F475" s="9"/>
+      <c r="F475" s="7"/>
     </row>
     <row r="476">
-      <c r="F476" s="9"/>
+      <c r="F476" s="7"/>
     </row>
     <row r="477">
-      <c r="F477" s="9"/>
+      <c r="F477" s="7"/>
     </row>
     <row r="478">
-      <c r="F478" s="9"/>
+      <c r="F478" s="7"/>
     </row>
     <row r="479">
-      <c r="F479" s="9"/>
+      <c r="F479" s="7"/>
     </row>
     <row r="480">
-      <c r="F480" s="9"/>
+      <c r="F480" s="7"/>
     </row>
     <row r="481">
-      <c r="F481" s="9"/>
+      <c r="F481" s="7"/>
     </row>
     <row r="482">
-      <c r="F482" s="9"/>
+      <c r="F482" s="7"/>
     </row>
     <row r="483">
-      <c r="F483" s="9"/>
+      <c r="F483" s="7"/>
     </row>
     <row r="484">
-      <c r="F484" s="9"/>
+      <c r="F484" s="7"/>
     </row>
     <row r="485">
-      <c r="F485" s="9"/>
+      <c r="F485" s="7"/>
     </row>
     <row r="486">
-      <c r="F486" s="9"/>
+      <c r="F486" s="7"/>
     </row>
     <row r="487">
-      <c r="F487" s="9"/>
+      <c r="F487" s="7"/>
     </row>
     <row r="488">
-      <c r="F488" s="9"/>
+      <c r="F488" s="7"/>
     </row>
     <row r="489">
-      <c r="F489" s="9"/>
+      <c r="F489" s="7"/>
     </row>
     <row r="490">
-      <c r="F490" s="9"/>
+      <c r="F490" s="7"/>
     </row>
     <row r="491">
-      <c r="F491" s="9"/>
+      <c r="F491" s="7"/>
     </row>
     <row r="492">
-      <c r="F492" s="9"/>
+      <c r="F492" s="7"/>
     </row>
     <row r="493">
-      <c r="F493" s="9"/>
+      <c r="F493" s="7"/>
     </row>
     <row r="494">
-      <c r="F494" s="9"/>
+      <c r="F494" s="7"/>
     </row>
     <row r="495">
-      <c r="F495" s="9"/>
+      <c r="F495" s="7"/>
     </row>
     <row r="496">
-      <c r="F496" s="9"/>
+      <c r="F496" s="7"/>
     </row>
     <row r="497">
-      <c r="F497" s="9"/>
+      <c r="F497" s="7"/>
     </row>
     <row r="498">
-      <c r="F498" s="9"/>
+      <c r="F498" s="7"/>
     </row>
     <row r="499">
-      <c r="F499" s="9"/>
+      <c r="F499" s="7"/>
     </row>
     <row r="500">
-      <c r="F500" s="9"/>
+      <c r="F500" s="7"/>
     </row>
     <row r="501">
-      <c r="F501" s="9"/>
+      <c r="F501" s="7"/>
     </row>
     <row r="502">
-      <c r="F502" s="9"/>
+      <c r="F502" s="7"/>
     </row>
     <row r="503">
-      <c r="F503" s="9"/>
+      <c r="F503" s="7"/>
     </row>
     <row r="504">
-      <c r="F504" s="9"/>
+      <c r="F504" s="7"/>
     </row>
     <row r="505">
-      <c r="F505" s="9"/>
+      <c r="F505" s="7"/>
     </row>
     <row r="506">
-      <c r="F506" s="9"/>
+      <c r="F506" s="7"/>
     </row>
     <row r="507">
-      <c r="F507" s="9"/>
+      <c r="F507" s="7"/>
     </row>
     <row r="508">
-      <c r="F508" s="9"/>
+      <c r="F508" s="7"/>
     </row>
     <row r="509">
-      <c r="F509" s="9"/>
+      <c r="F509" s="7"/>
     </row>
     <row r="510">
-      <c r="F510" s="9"/>
+      <c r="F510" s="7"/>
     </row>
     <row r="511">
-      <c r="F511" s="9"/>
+      <c r="F511" s="7"/>
     </row>
     <row r="512">
-      <c r="F512" s="9"/>
+      <c r="F512" s="7"/>
     </row>
     <row r="513">
-      <c r="F513" s="9"/>
+      <c r="F513" s="7"/>
     </row>
     <row r="514">
-      <c r="F514" s="9"/>
+      <c r="F514" s="7"/>
     </row>
     <row r="515">
-      <c r="F515" s="9"/>
+      <c r="F515" s="7"/>
     </row>
     <row r="516">
-      <c r="F516" s="9"/>
+      <c r="F516" s="7"/>
     </row>
     <row r="517">
-      <c r="F517" s="9"/>
+      <c r="F517" s="7"/>
     </row>
     <row r="518">
-      <c r="F518" s="9"/>
+      <c r="F518" s="7"/>
     </row>
     <row r="519">
-      <c r="F519" s="9"/>
+      <c r="F519" s="7"/>
     </row>
     <row r="520">
-      <c r="F520" s="9"/>
+      <c r="F520" s="7"/>
     </row>
     <row r="521">
-      <c r="F521" s="9"/>
+      <c r="F521" s="7"/>
     </row>
     <row r="522">
-      <c r="F522" s="9"/>
+      <c r="F522" s="7"/>
     </row>
     <row r="523">
-      <c r="F523" s="9"/>
+      <c r="F523" s="7"/>
     </row>
     <row r="524">
-      <c r="F524" s="9"/>
+      <c r="F524" s="7"/>
     </row>
     <row r="525">
-      <c r="F525" s="9"/>
+      <c r="F525" s="7"/>
     </row>
     <row r="526">
-      <c r="F526" s="9"/>
+      <c r="F526" s="7"/>
     </row>
     <row r="527">
-      <c r="F527" s="9"/>
+      <c r="F527" s="7"/>
     </row>
     <row r="528">
-      <c r="F528" s="9"/>
+      <c r="F528" s="7"/>
     </row>
     <row r="529">
-      <c r="F529" s="9"/>
+      <c r="F529" s="7"/>
     </row>
     <row r="530">
-      <c r="F530" s="9"/>
+      <c r="F530" s="7"/>
     </row>
     <row r="531">
-      <c r="F531" s="9"/>
+      <c r="F531" s="7"/>
     </row>
     <row r="532">
-      <c r="F532" s="9"/>
+      <c r="F532" s="7"/>
     </row>
     <row r="533">
-      <c r="F533" s="9"/>
+      <c r="F533" s="7"/>
     </row>
     <row r="534">
-      <c r="F534" s="9"/>
+      <c r="F534" s="7"/>
     </row>
     <row r="535">
-      <c r="F535" s="9"/>
+      <c r="F535" s="7"/>
     </row>
     <row r="536">
-      <c r="F536" s="9"/>
+      <c r="F536" s="7"/>
     </row>
     <row r="537">
-      <c r="F537" s="9"/>
+      <c r="F537" s="7"/>
     </row>
     <row r="538">
-      <c r="F538" s="9"/>
+      <c r="F538" s="7"/>
     </row>
     <row r="539">
-      <c r="F539" s="9"/>
+      <c r="F539" s="7"/>
     </row>
     <row r="540">
-      <c r="F540" s="9"/>
+      <c r="F540" s="7"/>
     </row>
     <row r="541">
-      <c r="F541" s="9"/>
+      <c r="F541" s="7"/>
     </row>
     <row r="542">
-      <c r="F542" s="9"/>
+      <c r="F542" s="7"/>
     </row>
     <row r="543">
-      <c r="F543" s="9"/>
+      <c r="F543" s="7"/>
     </row>
     <row r="544">
-      <c r="F544" s="9"/>
+      <c r="F544" s="7"/>
     </row>
     <row r="545">
-      <c r="F545" s="9"/>
+      <c r="F545" s="7"/>
     </row>
     <row r="546">
-      <c r="F546" s="9"/>
+      <c r="F546" s="7"/>
     </row>
     <row r="547">
-      <c r="F547" s="9"/>
+      <c r="F547" s="7"/>
     </row>
     <row r="548">
-      <c r="F548" s="9"/>
+      <c r="F548" s="7"/>
     </row>
     <row r="549">
-      <c r="F549" s="9"/>
+      <c r="F549" s="7"/>
     </row>
     <row r="550">
-      <c r="F550" s="9"/>
+      <c r="F550" s="7"/>
     </row>
     <row r="551">
-      <c r="F551" s="9"/>
+      <c r="F551" s="7"/>
     </row>
     <row r="552">
-      <c r="F552" s="9"/>
+      <c r="F552" s="7"/>
     </row>
     <row r="553">
-      <c r="F553" s="9"/>
+      <c r="F553" s="7"/>
     </row>
     <row r="554">
-      <c r="F554" s="9"/>
+      <c r="F554" s="7"/>
     </row>
     <row r="555">
-      <c r="F555" s="9"/>
+      <c r="F555" s="7"/>
     </row>
     <row r="556">
-      <c r="F556" s="9"/>
+      <c r="F556" s="7"/>
     </row>
     <row r="557">
-      <c r="F557" s="9"/>
+      <c r="F557" s="7"/>
     </row>
     <row r="558">
-      <c r="F558" s="9"/>
+      <c r="F558" s="7"/>
     </row>
     <row r="559">
-      <c r="F559" s="9"/>
+      <c r="F559" s="7"/>
     </row>
     <row r="560">
-      <c r="F560" s="9"/>
+      <c r="F560" s="7"/>
     </row>
     <row r="561">
-      <c r="F561" s="9"/>
+      <c r="F561" s="7"/>
     </row>
     <row r="562">
-      <c r="F562" s="9"/>
+      <c r="F562" s="7"/>
     </row>
     <row r="563">
-      <c r="F563" s="9"/>
+      <c r="F563" s="7"/>
     </row>
     <row r="564">
-      <c r="F564" s="9"/>
+      <c r="F564" s="7"/>
     </row>
     <row r="565">
-      <c r="F565" s="9"/>
+      <c r="F565" s="7"/>
     </row>
     <row r="566">
-      <c r="F566" s="9"/>
+      <c r="F566" s="7"/>
     </row>
     <row r="567">
-      <c r="F567" s="9"/>
+      <c r="F567" s="7"/>
     </row>
     <row r="568">
-      <c r="F568" s="9"/>
+      <c r="F568" s="7"/>
     </row>
     <row r="569">
-      <c r="F569" s="9"/>
+      <c r="F569" s="7"/>
     </row>
     <row r="570">
-      <c r="F570" s="9"/>
+      <c r="F570" s="7"/>
     </row>
     <row r="571">
-      <c r="F571" s="9"/>
+      <c r="F571" s="7"/>
     </row>
     <row r="572">
-      <c r="F572" s="9"/>
+      <c r="F572" s="7"/>
     </row>
     <row r="573">
-      <c r="F573" s="9"/>
+      <c r="F573" s="7"/>
     </row>
     <row r="574">
-      <c r="F574" s="9"/>
+      <c r="F574" s="7"/>
     </row>
     <row r="575">
-      <c r="F575" s="9"/>
+      <c r="F575" s="7"/>
     </row>
     <row r="576">
-      <c r="F576" s="9"/>
+      <c r="F576" s="7"/>
     </row>
     <row r="577">
-      <c r="F577" s="9"/>
+      <c r="F577" s="7"/>
     </row>
     <row r="578">
-      <c r="F578" s="9"/>
+      <c r="F578" s="7"/>
     </row>
     <row r="579">
-      <c r="F579" s="9"/>
+      <c r="F579" s="7"/>
     </row>
     <row r="580">
-      <c r="F580" s="9"/>
+      <c r="F580" s="7"/>
     </row>
     <row r="581">
-      <c r="F581" s="9"/>
+      <c r="F581" s="7"/>
     </row>
     <row r="582">
-      <c r="F582" s="9"/>
+      <c r="F582" s="7"/>
     </row>
     <row r="583">
-      <c r="F583" s="9"/>
+      <c r="F583" s="7"/>
     </row>
     <row r="584">
-      <c r="F584" s="9"/>
+      <c r="F584" s="7"/>
     </row>
     <row r="585">
-      <c r="F585" s="9"/>
+      <c r="F585" s="7"/>
     </row>
     <row r="586">
-      <c r="F586" s="9"/>
+      <c r="F586" s="7"/>
     </row>
     <row r="587">
-      <c r="F587" s="9"/>
+      <c r="F587" s="7"/>
     </row>
     <row r="588">
-      <c r="F588" s="9"/>
+      <c r="F588" s="7"/>
     </row>
     <row r="589">
-      <c r="F589" s="9"/>
+      <c r="F589" s="7"/>
     </row>
     <row r="590">
-      <c r="F590" s="9"/>
+      <c r="F590" s="7"/>
     </row>
     <row r="591">
-      <c r="F591" s="9"/>
+      <c r="F591" s="7"/>
     </row>
     <row r="592">
-      <c r="F592" s="9"/>
+      <c r="F592" s="7"/>
     </row>
     <row r="593">
-      <c r="F593" s="9"/>
+      <c r="F593" s="7"/>
     </row>
     <row r="594">
-      <c r="F594" s="9"/>
+      <c r="F594" s="7"/>
     </row>
     <row r="595">
-      <c r="F595" s="9"/>
+      <c r="F595" s="7"/>
     </row>
     <row r="596">
-      <c r="F596" s="9"/>
+      <c r="F596" s="7"/>
     </row>
     <row r="597">
-      <c r="F597" s="9"/>
+      <c r="F597" s="7"/>
     </row>
     <row r="598">
-      <c r="F598" s="9"/>
+      <c r="F598" s="7"/>
     </row>
     <row r="599">
-      <c r="F599" s="9"/>
+      <c r="F599" s="7"/>
     </row>
     <row r="600">
-      <c r="F600" s="9"/>
+      <c r="F600" s="7"/>
     </row>
     <row r="601">
-      <c r="F601" s="9"/>
+      <c r="F601" s="7"/>
     </row>
     <row r="602">
-      <c r="F602" s="9"/>
+      <c r="F602" s="7"/>
     </row>
     <row r="603">
-      <c r="F603" s="9"/>
+      <c r="F603" s="7"/>
     </row>
     <row r="604">
-      <c r="F604" s="9"/>
+      <c r="F604" s="7"/>
     </row>
     <row r="605">
-      <c r="F605" s="9"/>
+      <c r="F605" s="7"/>
     </row>
     <row r="606">
-      <c r="F606" s="9"/>
+      <c r="F606" s="7"/>
     </row>
     <row r="607">
-      <c r="F607" s="9"/>
+      <c r="F607" s="7"/>
     </row>
     <row r="608">
-      <c r="F608" s="9"/>
+      <c r="F608" s="7"/>
     </row>
     <row r="609">
-      <c r="F609" s="9"/>
+      <c r="F609" s="7"/>
     </row>
     <row r="610">
-      <c r="F610" s="9"/>
+      <c r="F610" s="7"/>
     </row>
     <row r="611">
-      <c r="F611" s="9"/>
+      <c r="F611" s="7"/>
     </row>
     <row r="612">
-      <c r="F612" s="9"/>
+      <c r="F612" s="7"/>
     </row>
     <row r="613">
-      <c r="F613" s="9"/>
+      <c r="F613" s="7"/>
     </row>
     <row r="614">
-      <c r="F614" s="9"/>
+      <c r="F614" s="7"/>
     </row>
     <row r="615">
-      <c r="F615" s="9"/>
+      <c r="F615" s="7"/>
     </row>
     <row r="616">
-      <c r="F616" s="9"/>
+      <c r="F616" s="7"/>
     </row>
     <row r="617">
-      <c r="F617" s="9"/>
+      <c r="F617" s="7"/>
     </row>
     <row r="618">
-      <c r="F618" s="9"/>
+      <c r="F618" s="7"/>
     </row>
     <row r="619">
-      <c r="F619" s="9"/>
+      <c r="F619" s="7"/>
     </row>
     <row r="620">
-      <c r="F620" s="9"/>
+      <c r="F620" s="7"/>
     </row>
     <row r="621">
-      <c r="F621" s="9"/>
+      <c r="F621" s="7"/>
     </row>
     <row r="622">
-      <c r="F622" s="9"/>
+      <c r="F622" s="7"/>
     </row>
     <row r="623">
-      <c r="F623" s="9"/>
+      <c r="F623" s="7"/>
     </row>
     <row r="624">
-      <c r="F624" s="9"/>
+      <c r="F624" s="7"/>
     </row>
     <row r="625">
-      <c r="F625" s="9"/>
+      <c r="F625" s="7"/>
     </row>
     <row r="626">
-      <c r="F626" s="9"/>
+      <c r="F626" s="7"/>
     </row>
     <row r="627">
-      <c r="F627" s="9"/>
+      <c r="F627" s="7"/>
     </row>
     <row r="628">
-      <c r="F628" s="9"/>
+      <c r="F628" s="7"/>
     </row>
     <row r="629">
-      <c r="F629" s="9"/>
+      <c r="F629" s="7"/>
     </row>
     <row r="630">
-      <c r="F630" s="9"/>
+      <c r="F630" s="7"/>
     </row>
     <row r="631">
-      <c r="F631" s="9"/>
+      <c r="F631" s="7"/>
     </row>
     <row r="632">
-      <c r="F632" s="9"/>
+      <c r="F632" s="7"/>
     </row>
     <row r="633">
-      <c r="F633" s="9"/>
+      <c r="F633" s="7"/>
     </row>
     <row r="634">
-      <c r="F634" s="9"/>
+      <c r="F634" s="7"/>
     </row>
     <row r="635">
-      <c r="F635" s="9"/>
+      <c r="F635" s="7"/>
     </row>
     <row r="636">
-      <c r="F636" s="9"/>
+      <c r="F636" s="7"/>
     </row>
     <row r="637">
-      <c r="F637" s="9"/>
+      <c r="F637" s="7"/>
     </row>
     <row r="638">
-      <c r="F638" s="9"/>
+      <c r="F638" s="7"/>
     </row>
     <row r="639">
-      <c r="F639" s="9"/>
+      <c r="F639" s="7"/>
     </row>
     <row r="640">
-      <c r="F640" s="9"/>
+      <c r="F640" s="7"/>
     </row>
     <row r="641">
-      <c r="F641" s="9"/>
+      <c r="F641" s="7"/>
     </row>
     <row r="642">
-      <c r="F642" s="9"/>
+      <c r="F642" s="7"/>
     </row>
     <row r="643">
-      <c r="F643" s="9"/>
+      <c r="F643" s="7"/>
     </row>
     <row r="644">
-      <c r="F644" s="9"/>
+      <c r="F644" s="7"/>
     </row>
     <row r="645">
-      <c r="F645" s="9"/>
+      <c r="F645" s="7"/>
     </row>
     <row r="646">
-      <c r="F646" s="9"/>
+      <c r="F646" s="7"/>
     </row>
     <row r="647">
-      <c r="F647" s="9"/>
+      <c r="F647" s="7"/>
     </row>
     <row r="648">
-      <c r="F648" s="9"/>
+      <c r="F648" s="7"/>
     </row>
     <row r="649">
-      <c r="F649" s="9"/>
+      <c r="F649" s="7"/>
     </row>
     <row r="650">
-      <c r="F650" s="9"/>
+      <c r="F650" s="7"/>
     </row>
     <row r="651">
-      <c r="F651" s="9"/>
+      <c r="F651" s="7"/>
     </row>
     <row r="652">
-      <c r="F652" s="9"/>
+      <c r="F652" s="7"/>
     </row>
     <row r="653">
-      <c r="F653" s="9"/>
+      <c r="F653" s="7"/>
     </row>
     <row r="654">
-      <c r="F654" s="9"/>
+      <c r="F654" s="7"/>
     </row>
     <row r="655">
-      <c r="F655" s="9"/>
+      <c r="F655" s="7"/>
     </row>
     <row r="656">
-      <c r="F656" s="9"/>
+      <c r="F656" s="7"/>
     </row>
     <row r="657">
-      <c r="F657" s="9"/>
+      <c r="F657" s="7"/>
     </row>
     <row r="658">
-      <c r="F658" s="9"/>
+      <c r="F658" s="7"/>
     </row>
     <row r="659">
-      <c r="F659" s="9"/>
+      <c r="F659" s="7"/>
     </row>
     <row r="660">
-      <c r="F660" s="9"/>
+      <c r="F660" s="7"/>
     </row>
     <row r="661">
-      <c r="F661" s="9"/>
+      <c r="F661" s="7"/>
     </row>
     <row r="662">
-      <c r="F662" s="9"/>
+      <c r="F662" s="7"/>
     </row>
     <row r="663">
-      <c r="F663" s="9"/>
+      <c r="F663" s="7"/>
     </row>
     <row r="664">
-      <c r="F664" s="9"/>
+      <c r="F664" s="7"/>
     </row>
     <row r="665">
-      <c r="F665" s="9"/>
+      <c r="F665" s="7"/>
     </row>
     <row r="666">
-      <c r="F666" s="9"/>
+      <c r="F666" s="7"/>
     </row>
     <row r="667">
-      <c r="F667" s="9"/>
+      <c r="F667" s="7"/>
     </row>
     <row r="668">
-      <c r="F668" s="9"/>
+      <c r="F668" s="7"/>
     </row>
     <row r="669">
-      <c r="F669" s="9"/>
+      <c r="F669" s="7"/>
     </row>
     <row r="670">
-      <c r="F670" s="9"/>
+      <c r="F670" s="7"/>
     </row>
     <row r="671">
-      <c r="F671" s="9"/>
+      <c r="F671" s="7"/>
     </row>
     <row r="672">
-      <c r="F672" s="9"/>
+      <c r="F672" s="7"/>
     </row>
     <row r="673">
-      <c r="F673" s="9"/>
+      <c r="F673" s="7"/>
     </row>
     <row r="674">
-      <c r="F674" s="9"/>
+      <c r="F674" s="7"/>
     </row>
     <row r="675">
-      <c r="F675" s="9"/>
+      <c r="F675" s="7"/>
     </row>
     <row r="676">
-      <c r="F676" s="9"/>
+      <c r="F676" s="7"/>
     </row>
     <row r="677">
-      <c r="F677" s="9"/>
+      <c r="F677" s="7"/>
     </row>
     <row r="678">
-      <c r="F678" s="9"/>
+      <c r="F678" s="7"/>
     </row>
     <row r="679">
-      <c r="F679" s="9"/>
+      <c r="F679" s="7"/>
     </row>
     <row r="680">
-      <c r="F680" s="9"/>
+      <c r="F680" s="7"/>
     </row>
     <row r="681">
-      <c r="F681" s="9"/>
+      <c r="F681" s="7"/>
     </row>
     <row r="682">
-      <c r="F682" s="9"/>
+      <c r="F682" s="7"/>
     </row>
     <row r="683">
-      <c r="F683" s="9"/>
+      <c r="F683" s="7"/>
     </row>
     <row r="684">
-      <c r="F684" s="9"/>
+      <c r="F684" s="7"/>
     </row>
     <row r="685">
-      <c r="F685" s="9"/>
+      <c r="F685" s="7"/>
     </row>
     <row r="686">
-      <c r="F686" s="9"/>
+      <c r="F686" s="7"/>
     </row>
     <row r="687">
-      <c r="F687" s="9"/>
+      <c r="F687" s="7"/>
     </row>
     <row r="688">
-      <c r="F688" s="9"/>
+      <c r="F688" s="7"/>
     </row>
     <row r="689">
-      <c r="F689" s="9"/>
+      <c r="F689" s="7"/>
     </row>
     <row r="690">
-      <c r="F690" s="9"/>
+      <c r="F690" s="7"/>
     </row>
     <row r="691">
-      <c r="F691" s="9"/>
+      <c r="F691" s="7"/>
     </row>
     <row r="692">
-      <c r="F692" s="9"/>
+      <c r="F692" s="7"/>
     </row>
     <row r="693">
-      <c r="F693" s="9"/>
+      <c r="F693" s="7"/>
     </row>
     <row r="694">
-      <c r="F694" s="9"/>
+      <c r="F694" s="7"/>
     </row>
     <row r="695">
-      <c r="F695" s="9"/>
+      <c r="F695" s="7"/>
     </row>
     <row r="696">
-      <c r="F696" s="9"/>
+      <c r="F696" s="7"/>
     </row>
     <row r="697">
-      <c r="F697" s="9"/>
+      <c r="F697" s="7"/>
     </row>
     <row r="698">
-      <c r="F698" s="9"/>
+      <c r="F698" s="7"/>
     </row>
     <row r="699">
-      <c r="F699" s="9"/>
+      <c r="F699" s="7"/>
     </row>
     <row r="700">
-      <c r="F700" s="9"/>
+      <c r="F700" s="7"/>
     </row>
     <row r="701">
-      <c r="F701" s="9"/>
+      <c r="F701" s="7"/>
     </row>
     <row r="702">
-      <c r="F702" s="9"/>
+      <c r="F702" s="7"/>
     </row>
     <row r="703">
-      <c r="F703" s="9"/>
+      <c r="F703" s="7"/>
     </row>
     <row r="704">
-      <c r="F704" s="9"/>
+      <c r="F704" s="7"/>
     </row>
     <row r="705">
-      <c r="F705" s="9"/>
+      <c r="F705" s="7"/>
     </row>
     <row r="706">
-      <c r="F706" s="9"/>
+      <c r="F706" s="7"/>
     </row>
     <row r="707">
-      <c r="F707" s="9"/>
+      <c r="F707" s="7"/>
     </row>
     <row r="708">
-      <c r="F708" s="9"/>
+      <c r="F708" s="7"/>
     </row>
     <row r="709">
-      <c r="F709" s="9"/>
+      <c r="F709" s="7"/>
     </row>
     <row r="710">
-      <c r="F710" s="9"/>
+      <c r="F710" s="7"/>
     </row>
     <row r="711">
-      <c r="F711" s="9"/>
+      <c r="F711" s="7"/>
     </row>
     <row r="712">
-      <c r="F712" s="9"/>
+      <c r="F712" s="7"/>
     </row>
     <row r="713">
-      <c r="F713" s="9"/>
+      <c r="F713" s="7"/>
     </row>
     <row r="714">
-      <c r="F714" s="9"/>
+      <c r="F714" s="7"/>
     </row>
     <row r="715">
-      <c r="F715" s="9"/>
+      <c r="F715" s="7"/>
     </row>
     <row r="716">
-      <c r="F716" s="9"/>
+      <c r="F716" s="7"/>
     </row>
     <row r="717">
-      <c r="F717" s="9"/>
+      <c r="F717" s="7"/>
     </row>
     <row r="718">
-      <c r="F718" s="9"/>
+      <c r="F718" s="7"/>
     </row>
     <row r="719">
-      <c r="F719" s="9"/>
+      <c r="F719" s="7"/>
     </row>
     <row r="720">
-      <c r="F720" s="9"/>
+      <c r="F720" s="7"/>
     </row>
     <row r="721">
-      <c r="F721" s="9"/>
+      <c r="F721" s="7"/>
     </row>
     <row r="722">
-      <c r="F722" s="9"/>
+      <c r="F722" s="7"/>
     </row>
     <row r="723">
-      <c r="F723" s="9"/>
+      <c r="F723" s="7"/>
     </row>
     <row r="724">
-      <c r="F724" s="9"/>
+      <c r="F724" s="7"/>
     </row>
     <row r="725">
-      <c r="F725" s="9"/>
+      <c r="F725" s="7"/>
     </row>
     <row r="726">
-      <c r="F726" s="9"/>
+      <c r="F726" s="7"/>
     </row>
     <row r="727">
-      <c r="F727" s="9"/>
+      <c r="F727" s="7"/>
     </row>
     <row r="728">
-      <c r="F728" s="9"/>
+      <c r="F728" s="7"/>
     </row>
     <row r="729">
-      <c r="F729" s="9"/>
+      <c r="F729" s="7"/>
     </row>
     <row r="730">
-      <c r="F730" s="9"/>
+      <c r="F730" s="7"/>
     </row>
     <row r="731">
-      <c r="F731" s="9"/>
+      <c r="F731" s="7"/>
     </row>
     <row r="732">
-      <c r="F732" s="9"/>
+      <c r="F732" s="7"/>
     </row>
     <row r="733">
-      <c r="F733" s="9"/>
+      <c r="F733" s="7"/>
     </row>
     <row r="734">
-      <c r="F734" s="9"/>
+      <c r="F734" s="7"/>
     </row>
     <row r="735">
-      <c r="F735" s="9"/>
+      <c r="F735" s="7"/>
     </row>
     <row r="736">
-      <c r="F736" s="9"/>
+      <c r="F736" s="7"/>
     </row>
     <row r="737">
-      <c r="F737" s="9"/>
+      <c r="F737" s="7"/>
     </row>
     <row r="738">
-      <c r="F738" s="9"/>
+      <c r="F738" s="7"/>
     </row>
     <row r="739">
-      <c r="F739" s="9"/>
+      <c r="F739" s="7"/>
     </row>
     <row r="740">
-      <c r="F740" s="9"/>
+      <c r="F740" s="7"/>
     </row>
     <row r="741">
-      <c r="F741" s="9"/>
+      <c r="F741" s="7"/>
     </row>
     <row r="742">
-      <c r="F742" s="9"/>
+      <c r="F742" s="7"/>
     </row>
     <row r="743">
-      <c r="F743" s="9"/>
+      <c r="F743" s="7"/>
     </row>
     <row r="744">
-      <c r="F744" s="9"/>
+      <c r="F744" s="7"/>
     </row>
     <row r="745">
-      <c r="F745" s="9"/>
+      <c r="F745" s="7"/>
     </row>
     <row r="746">
-      <c r="F746" s="9"/>
+      <c r="F746" s="7"/>
     </row>
     <row r="747">
-      <c r="F747" s="9"/>
+      <c r="F747" s="7"/>
     </row>
     <row r="748">
-      <c r="F748" s="9"/>
+      <c r="F748" s="7"/>
     </row>
     <row r="749">
-      <c r="F749" s="9"/>
+      <c r="F749" s="7"/>
     </row>
     <row r="750">
-      <c r="F750" s="9"/>
+      <c r="F750" s="7"/>
     </row>
     <row r="751">
-      <c r="F751" s="9"/>
+      <c r="F751" s="7"/>
     </row>
     <row r="752">
-      <c r="F752" s="9"/>
+      <c r="F752" s="7"/>
     </row>
     <row r="753">
-      <c r="F753" s="9"/>
+      <c r="F753" s="7"/>
     </row>
     <row r="754">
-      <c r="F754" s="9"/>
+      <c r="F754" s="7"/>
     </row>
     <row r="755">
-      <c r="F755" s="9"/>
+      <c r="F755" s="7"/>
     </row>
     <row r="756">
-      <c r="F756" s="9"/>
+      <c r="F756" s="7"/>
     </row>
     <row r="757">
-      <c r="F757" s="9"/>
+      <c r="F757" s="7"/>
     </row>
     <row r="758">
-      <c r="F758" s="9"/>
+      <c r="F758" s="7"/>
     </row>
     <row r="759">
-      <c r="F759" s="9"/>
+      <c r="F759" s="7"/>
     </row>
     <row r="760">
-      <c r="F760" s="9"/>
+      <c r="F760" s="7"/>
     </row>
     <row r="761">
-      <c r="F761" s="9"/>
+      <c r="F761" s="7"/>
     </row>
     <row r="762">
-      <c r="F762" s="9"/>
+      <c r="F762" s="7"/>
     </row>
     <row r="763">
-      <c r="F763" s="9"/>
+      <c r="F763" s="7"/>
     </row>
     <row r="764">
-      <c r="F764" s="9"/>
+      <c r="F764" s="7"/>
     </row>
     <row r="765">
-      <c r="F765" s="9"/>
+      <c r="F765" s="7"/>
     </row>
     <row r="766">
-      <c r="F766" s="9"/>
+      <c r="F766" s="7"/>
     </row>
     <row r="767">
-      <c r="F767" s="9"/>
+      <c r="F767" s="7"/>
     </row>
     <row r="768">
-      <c r="F768" s="9"/>
+      <c r="F768" s="7"/>
     </row>
     <row r="769">
-      <c r="F769" s="9"/>
+      <c r="F769" s="7"/>
     </row>
     <row r="770">
-      <c r="F770" s="9"/>
+      <c r="F770" s="7"/>
     </row>
     <row r="771">
-      <c r="F771" s="9"/>
+      <c r="F771" s="7"/>
     </row>
     <row r="772">
-      <c r="F772" s="9"/>
+      <c r="F772" s="7"/>
     </row>
     <row r="773">
-      <c r="F773" s="9"/>
+      <c r="F773" s="7"/>
     </row>
     <row r="774">
-      <c r="F774" s="9"/>
+      <c r="F774" s="7"/>
     </row>
     <row r="775">
-      <c r="F775" s="9"/>
+      <c r="F775" s="7"/>
     </row>
     <row r="776">
-      <c r="F776" s="9"/>
+      <c r="F776" s="7"/>
     </row>
     <row r="777">
-      <c r="F777" s="9"/>
+      <c r="F777" s="7"/>
     </row>
     <row r="778">
-      <c r="F778" s="9"/>
+      <c r="F778" s="7"/>
     </row>
     <row r="779">
-      <c r="F779" s="9"/>
+      <c r="F779" s="7"/>
     </row>
     <row r="780">
-      <c r="F780" s="9"/>
+      <c r="F780" s="7"/>
     </row>
     <row r="781">
-      <c r="F781" s="9"/>
+      <c r="F781" s="7"/>
     </row>
     <row r="782">
-      <c r="F782" s="9"/>
+      <c r="F782" s="7"/>
     </row>
     <row r="783">
-      <c r="F783" s="9"/>
+      <c r="F783" s="7"/>
     </row>
     <row r="784">
-      <c r="F784" s="9"/>
+      <c r="F784" s="7"/>
     </row>
     <row r="785">
-      <c r="F785" s="9"/>
+      <c r="F785" s="7"/>
     </row>
     <row r="786">
-      <c r="F786" s="9"/>
+      <c r="F786" s="7"/>
     </row>
     <row r="787">
-      <c r="F787" s="9"/>
+      <c r="F787" s="7"/>
     </row>
     <row r="788">
-      <c r="F788" s="9"/>
+      <c r="F788" s="7"/>
     </row>
     <row r="789">
-      <c r="F789" s="9"/>
+      <c r="F789" s="7"/>
     </row>
     <row r="790">
-      <c r="F790" s="9"/>
+      <c r="F790" s="7"/>
     </row>
     <row r="791">
-      <c r="F791" s="9"/>
+      <c r="F791" s="7"/>
     </row>
     <row r="792">
-      <c r="F792" s="9"/>
+      <c r="F792" s="7"/>
     </row>
     <row r="793">
-      <c r="F793" s="9"/>
+      <c r="F793" s="7"/>
     </row>
     <row r="794">
-      <c r="F794" s="9"/>
+      <c r="F794" s="7"/>
     </row>
     <row r="795">
-      <c r="F795" s="9"/>
+      <c r="F795" s="7"/>
     </row>
     <row r="796">
-      <c r="F796" s="9"/>
+      <c r="F796" s="7"/>
     </row>
     <row r="797">
-      <c r="F797" s="9"/>
+      <c r="F797" s="7"/>
     </row>
     <row r="798">
-      <c r="F798" s="9"/>
+      <c r="F798" s="7"/>
     </row>
     <row r="799">
-      <c r="F799" s="9"/>
+      <c r="F799" s="7"/>
     </row>
     <row r="800">
-      <c r="F800" s="9"/>
+      <c r="F800" s="7"/>
     </row>
     <row r="801">
-      <c r="F801" s="9"/>
+      <c r="F801" s="7"/>
     </row>
     <row r="802">
-      <c r="F802" s="9"/>
+      <c r="F802" s="7"/>
     </row>
     <row r="803">
-      <c r="F803" s="9"/>
+      <c r="F803" s="7"/>
     </row>
     <row r="804">
-      <c r="F804" s="9"/>
+      <c r="F804" s="7"/>
     </row>
     <row r="805">
-      <c r="F805" s="9"/>
+      <c r="F805" s="7"/>
     </row>
     <row r="806">
-      <c r="F806" s="9"/>
+      <c r="F806" s="7"/>
     </row>
     <row r="807">
-      <c r="F807" s="9"/>
+      <c r="F807" s="7"/>
     </row>
     <row r="808">
-      <c r="F808" s="9"/>
+      <c r="F808" s="7"/>
     </row>
     <row r="809">
-      <c r="F809" s="9"/>
+      <c r="F809" s="7"/>
     </row>
     <row r="810">
-      <c r="F810" s="9"/>
+      <c r="F810" s="7"/>
     </row>
     <row r="811">
-      <c r="F811" s="9"/>
+      <c r="F811" s="7"/>
     </row>
     <row r="812">
-      <c r="F812" s="9"/>
+      <c r="F812" s="7"/>
     </row>
     <row r="813">
-      <c r="F813" s="9"/>
+      <c r="F813" s="7"/>
     </row>
     <row r="814">
-      <c r="F814" s="9"/>
+      <c r="F814" s="7"/>
     </row>
     <row r="815">
-      <c r="F815" s="9"/>
+      <c r="F815" s="7"/>
     </row>
     <row r="816">
-      <c r="F816" s="9"/>
+      <c r="F816" s="7"/>
     </row>
     <row r="817">
-      <c r="F817" s="9"/>
+      <c r="F817" s="7"/>
     </row>
     <row r="818">
-      <c r="F818" s="9"/>
+      <c r="F818" s="7"/>
     </row>
     <row r="819">
-      <c r="F819" s="9"/>
+      <c r="F819" s="7"/>
     </row>
     <row r="820">
-      <c r="F820" s="9"/>
+      <c r="F820" s="7"/>
     </row>
     <row r="821">
-      <c r="F821" s="9"/>
+      <c r="F821" s="7"/>
     </row>
     <row r="822">
-      <c r="F822" s="9"/>
+      <c r="F822" s="7"/>
     </row>
     <row r="823">
-      <c r="F823" s="9"/>
+      <c r="F823" s="7"/>
     </row>
     <row r="824">
-      <c r="F824" s="9"/>
+      <c r="F824" s="7"/>
     </row>
     <row r="825">
-      <c r="F825" s="9"/>
+      <c r="F825" s="7"/>
     </row>
     <row r="826">
-      <c r="F826" s="9"/>
+      <c r="F826" s="7"/>
     </row>
     <row r="827">
-      <c r="F827" s="9"/>
+      <c r="F827" s="7"/>
     </row>
     <row r="828">
-      <c r="F828" s="9"/>
+      <c r="F828" s="7"/>
     </row>
     <row r="829">
-      <c r="F829" s="9"/>
+      <c r="F829" s="7"/>
     </row>
     <row r="830">
-      <c r="F830" s="9"/>
+      <c r="F830" s="7"/>
     </row>
     <row r="831">
-      <c r="F831" s="9"/>
+      <c r="F831" s="7"/>
     </row>
     <row r="832">
-      <c r="F832" s="9"/>
+      <c r="F832" s="7"/>
     </row>
     <row r="833">
-      <c r="F833" s="9"/>
+      <c r="F833" s="7"/>
     </row>
     <row r="834">
-      <c r="F834" s="9"/>
+      <c r="F834" s="7"/>
     </row>
     <row r="835">
-      <c r="F835" s="9"/>
+      <c r="F835" s="7"/>
     </row>
     <row r="836">
-      <c r="F836" s="9"/>
+      <c r="F836" s="7"/>
     </row>
     <row r="837">
-      <c r="F837" s="9"/>
+      <c r="F837" s="7"/>
     </row>
     <row r="838">
-      <c r="F838" s="9"/>
+      <c r="F838" s="7"/>
     </row>
     <row r="839">
-      <c r="F839" s="9"/>
+      <c r="F839" s="7"/>
     </row>
     <row r="840">
-      <c r="F840" s="9"/>
+      <c r="F840" s="7"/>
     </row>
     <row r="841">
-      <c r="F841" s="9"/>
+      <c r="F841" s="7"/>
     </row>
     <row r="842">
-      <c r="F842" s="9"/>
+      <c r="F842" s="7"/>
     </row>
     <row r="843">
-      <c r="F843" s="9"/>
+      <c r="F843" s="7"/>
     </row>
     <row r="844">
-      <c r="F844" s="9"/>
+      <c r="F844" s="7"/>
     </row>
     <row r="845">
-      <c r="F845" s="9"/>
+      <c r="F845" s="7"/>
     </row>
     <row r="846">
-      <c r="F846" s="9"/>
+      <c r="F846" s="7"/>
     </row>
     <row r="847">
-      <c r="F847" s="9"/>
+      <c r="F847" s="7"/>
     </row>
     <row r="848">
-      <c r="F848" s="9"/>
+      <c r="F848" s="7"/>
     </row>
     <row r="849">
-      <c r="F849" s="9"/>
+      <c r="F849" s="7"/>
     </row>
     <row r="850">
-      <c r="F850" s="9"/>
+      <c r="F850" s="7"/>
     </row>
     <row r="851">
-      <c r="F851" s="9"/>
+      <c r="F851" s="7"/>
     </row>
     <row r="852">
-      <c r="F852" s="9"/>
+      <c r="F852" s="7"/>
     </row>
     <row r="853">
-      <c r="F853" s="9"/>
+      <c r="F853" s="7"/>
     </row>
     <row r="854">
-      <c r="F854" s="9"/>
+      <c r="F854" s="7"/>
     </row>
     <row r="855">
-      <c r="F855" s="9"/>
+      <c r="F855" s="7"/>
     </row>
     <row r="856">
-      <c r="F856" s="9"/>
+      <c r="F856" s="7"/>
     </row>
     <row r="857">
-      <c r="F857" s="9"/>
+      <c r="F857" s="7"/>
     </row>
     <row r="858">
-      <c r="F858" s="9"/>
+      <c r="F858" s="7"/>
     </row>
     <row r="859">
-      <c r="F859" s="9"/>
+      <c r="F859" s="7"/>
     </row>
     <row r="860">
-      <c r="F860" s="9"/>
+      <c r="F860" s="7"/>
     </row>
     <row r="861">
-      <c r="F861" s="9"/>
+      <c r="F861" s="7"/>
     </row>
     <row r="862">
-      <c r="F862" s="9"/>
+      <c r="F862" s="7"/>
     </row>
     <row r="863">
-      <c r="F863" s="9"/>
+      <c r="F863" s="7"/>
     </row>
     <row r="864">
-      <c r="F864" s="9"/>
+      <c r="F864" s="7"/>
     </row>
     <row r="865">
-      <c r="F865" s="9"/>
+      <c r="F865" s="7"/>
     </row>
     <row r="866">
-      <c r="F866" s="9"/>
+      <c r="F866" s="7"/>
     </row>
     <row r="867">
-      <c r="F867" s="9"/>
+      <c r="F867" s="7"/>
     </row>
     <row r="868">
-      <c r="F868" s="9"/>
+      <c r="F868" s="7"/>
     </row>
     <row r="869">
-      <c r="F869" s="9"/>
+      <c r="F869" s="7"/>
     </row>
     <row r="870">
-      <c r="F870" s="9"/>
+      <c r="F870" s="7"/>
     </row>
     <row r="871">
-      <c r="F871" s="9"/>
+      <c r="F871" s="7"/>
     </row>
     <row r="872">
-      <c r="F872" s="9"/>
+      <c r="F872" s="7"/>
     </row>
     <row r="873">
-      <c r="F873" s="9"/>
+      <c r="F873" s="7"/>
     </row>
     <row r="874">
-      <c r="F874" s="9"/>
+      <c r="F874" s="7"/>
     </row>
     <row r="875">
-      <c r="F875" s="9"/>
+      <c r="F875" s="7"/>
     </row>
     <row r="876">
-      <c r="F876" s="9"/>
+      <c r="F876" s="7"/>
     </row>
     <row r="877">
-      <c r="F877" s="9"/>
+      <c r="F877" s="7"/>
     </row>
     <row r="878">
-      <c r="F878" s="9"/>
+      <c r="F878" s="7"/>
     </row>
     <row r="879">
-      <c r="F879" s="9"/>
+      <c r="F879" s="7"/>
     </row>
     <row r="880">
-      <c r="F880" s="9"/>
+      <c r="F880" s="7"/>
     </row>
     <row r="881">
-      <c r="F881" s="9"/>
+      <c r="F881" s="7"/>
     </row>
     <row r="882">
-      <c r="F882" s="9"/>
+      <c r="F882" s="7"/>
     </row>
     <row r="883">
-      <c r="F883" s="9"/>
+      <c r="F883" s="7"/>
     </row>
     <row r="884">
-      <c r="F884" s="9"/>
+      <c r="F884" s="7"/>
     </row>
     <row r="885">
-      <c r="F885" s="9"/>
+      <c r="F885" s="7"/>
     </row>
     <row r="886">
-      <c r="F886" s="9"/>
+      <c r="F886" s="7"/>
     </row>
     <row r="887">
-      <c r="F887" s="9"/>
+      <c r="F887" s="7"/>
     </row>
     <row r="888">
-      <c r="F888" s="9"/>
+      <c r="F888" s="7"/>
     </row>
     <row r="889">
-      <c r="F889" s="9"/>
+      <c r="F889" s="7"/>
     </row>
     <row r="890">
-      <c r="F890" s="9"/>
+      <c r="F890" s="7"/>
     </row>
     <row r="891">
-      <c r="F891" s="9"/>
+      <c r="F891" s="7"/>
     </row>
     <row r="892">
-      <c r="F892" s="9"/>
+      <c r="F892" s="7"/>
     </row>
     <row r="893">
-      <c r="F893" s="9"/>
+      <c r="F893" s="7"/>
     </row>
     <row r="894">
-      <c r="F894" s="9"/>
+      <c r="F894" s="7"/>
     </row>
     <row r="895">
-      <c r="F895" s="9"/>
+      <c r="F895" s="7"/>
     </row>
     <row r="896">
-      <c r="F896" s="9"/>
+      <c r="F896" s="7"/>
     </row>
     <row r="897">
-      <c r="F897" s="9"/>
+      <c r="F897" s="7"/>
     </row>
     <row r="898">
-      <c r="F898" s="9"/>
+      <c r="F898" s="7"/>
     </row>
     <row r="899">
-      <c r="F899" s="9"/>
+      <c r="F899" s="7"/>
     </row>
     <row r="900">
-      <c r="F900" s="9"/>
+      <c r="F900" s="7"/>
     </row>
     <row r="901">
-      <c r="F901" s="9"/>
+      <c r="F901" s="7"/>
     </row>
     <row r="902">
-      <c r="F902" s="9"/>
+      <c r="F902" s="7"/>
     </row>
     <row r="903">
-      <c r="F903" s="9"/>
+      <c r="F903" s="7"/>
     </row>
     <row r="904">
-      <c r="F904" s="9"/>
+      <c r="F904" s="7"/>
     </row>
     <row r="905">
-      <c r="F905" s="9"/>
+      <c r="F905" s="7"/>
     </row>
     <row r="906">
-      <c r="F906" s="9"/>
+      <c r="F906" s="7"/>
     </row>
     <row r="907">
-      <c r="F907" s="9"/>
+      <c r="F907" s="7"/>
     </row>
     <row r="908">
-      <c r="F908" s="9"/>
+      <c r="F908" s="7"/>
     </row>
     <row r="909">
-      <c r="F909" s="9"/>
+      <c r="F909" s="7"/>
     </row>
     <row r="910">
-      <c r="F910" s="9"/>
+      <c r="F910" s="7"/>
     </row>
     <row r="911">
-      <c r="F911" s="9"/>
+      <c r="F911" s="7"/>
     </row>
     <row r="912">
-      <c r="F912" s="9"/>
+      <c r="F912" s="7"/>
     </row>
     <row r="913">
-      <c r="F913" s="9"/>
+      <c r="F913" s="7"/>
     </row>
     <row r="914">
-      <c r="F914" s="9"/>
+      <c r="F914" s="7"/>
     </row>
     <row r="915">
-      <c r="F915" s="9"/>
+      <c r="F915" s="7"/>
     </row>
     <row r="916">
-      <c r="F916" s="9"/>
+      <c r="F916" s="7"/>
     </row>
     <row r="917">
-      <c r="F917" s="9"/>
+      <c r="F917" s="7"/>
     </row>
     <row r="918">
-      <c r="F918" s="9"/>
+      <c r="F918" s="7"/>
     </row>
     <row r="919">
-      <c r="F919" s="9"/>
+      <c r="F919" s="7"/>
     </row>
     <row r="920">
-      <c r="F920" s="9"/>
+      <c r="F920" s="7"/>
     </row>
     <row r="921">
-      <c r="F921" s="9"/>
+      <c r="F921" s="7"/>
     </row>
     <row r="922">
-      <c r="F922" s="9"/>
+      <c r="F922" s="7"/>
     </row>
     <row r="923">
-      <c r="F923" s="9"/>
+      <c r="F923" s="7"/>
     </row>
     <row r="924">
-      <c r="F924" s="9"/>
+      <c r="F924" s="7"/>
     </row>
     <row r="925">
-      <c r="F925" s="9"/>
+      <c r="F925" s="7"/>
     </row>
     <row r="926">
-      <c r="F926" s="9"/>
+      <c r="F926" s="7"/>
     </row>
     <row r="927">
-      <c r="F927" s="9"/>
+      <c r="F927" s="7"/>
     </row>
     <row r="928">
-      <c r="F928" s="9"/>
+      <c r="F928" s="7"/>
     </row>
     <row r="929">
-      <c r="F929" s="9"/>
+      <c r="F929" s="7"/>
     </row>
     <row r="930">
-      <c r="F930" s="9"/>
+      <c r="F930" s="7"/>
     </row>
     <row r="931">
-      <c r="F931" s="9"/>
+      <c r="F931" s="7"/>
     </row>
     <row r="932">
-      <c r="F932" s="9"/>
+      <c r="F932" s="7"/>
     </row>
     <row r="933">
-      <c r="F933" s="9"/>
+      <c r="F933" s="7"/>
     </row>
     <row r="934">
-      <c r="F934" s="9"/>
+      <c r="F934" s="7"/>
     </row>
     <row r="935">
-      <c r="F935" s="9"/>
+      <c r="F935" s="7"/>
     </row>
     <row r="936">
-      <c r="F936" s="9"/>
+      <c r="F936" s="7"/>
     </row>
     <row r="937">
-      <c r="F937" s="9"/>
+      <c r="F937" s="7"/>
     </row>
     <row r="938">
-      <c r="F938" s="9"/>
+      <c r="F938" s="7"/>
     </row>
     <row r="939">
-      <c r="F939" s="9"/>
+      <c r="F939" s="7"/>
     </row>
     <row r="940">
-      <c r="F940" s="9"/>
+      <c r="F940" s="7"/>
     </row>
     <row r="941">
-      <c r="F941" s="9"/>
+      <c r="F941" s="7"/>
     </row>
     <row r="942">
-      <c r="F942" s="9"/>
+      <c r="F942" s="7"/>
     </row>
     <row r="943">
-      <c r="F943" s="9"/>
+      <c r="F943" s="7"/>
     </row>
     <row r="944">
-      <c r="F944" s="9"/>
+      <c r="F944" s="7"/>
     </row>
     <row r="945">
-      <c r="F945" s="9"/>
+      <c r="F945" s="7"/>
     </row>
     <row r="946">
-      <c r="F946" s="9"/>
+      <c r="F946" s="7"/>
     </row>
     <row r="947">
-      <c r="F947" s="9"/>
+      <c r="F947" s="7"/>
     </row>
     <row r="948">
-      <c r="F948" s="9"/>
+      <c r="F948" s="7"/>
     </row>
     <row r="949">
-      <c r="F949" s="9"/>
+      <c r="F949" s="7"/>
     </row>
     <row r="950">
-      <c r="F950" s="9"/>
+      <c r="F950" s="7"/>
     </row>
     <row r="951">
-      <c r="F951" s="9"/>
+      <c r="F951" s="7"/>
     </row>
     <row r="952">
-      <c r="F952" s="9"/>
+      <c r="F952" s="7"/>
     </row>
     <row r="953">
-      <c r="F953" s="9"/>
+      <c r="F953" s="7"/>
     </row>
     <row r="954">
-      <c r="F954" s="9"/>
+      <c r="F954" s="7"/>
     </row>
     <row r="955">
-      <c r="F955" s="9"/>
+      <c r="F955" s="7"/>
     </row>
     <row r="956">
-      <c r="F956" s="9"/>
+      <c r="F956" s="7"/>
     </row>
     <row r="957">
-      <c r="F957" s="9"/>
+      <c r="F957" s="7"/>
     </row>
     <row r="958">
-      <c r="F958" s="9"/>
+      <c r="F958" s="7"/>
     </row>
     <row r="959">
-      <c r="F959" s="9"/>
+      <c r="F959" s="7"/>
     </row>
     <row r="960">
-      <c r="F960" s="9"/>
+      <c r="F960" s="7"/>
     </row>
     <row r="961">
-      <c r="F961" s="9"/>
+      <c r="F961" s="7"/>
     </row>
     <row r="962">
-      <c r="F962" s="9"/>
+      <c r="F962" s="7"/>
     </row>
     <row r="963">
-      <c r="F963" s="9"/>
+      <c r="F963" s="7"/>
     </row>
     <row r="964">
-      <c r="F964" s="9"/>
+      <c r="F964" s="7"/>
     </row>
     <row r="965">
-      <c r="F965" s="9"/>
+      <c r="F965" s="7"/>
     </row>
     <row r="966">
-      <c r="F966" s="9"/>
+      <c r="F966" s="7"/>
     </row>
     <row r="967">
-      <c r="F967" s="9"/>
+      <c r="F967" s="7"/>
     </row>
     <row r="968">
-      <c r="F968" s="9"/>
+      <c r="F968" s="7"/>
     </row>
     <row r="969">
-      <c r="F969" s="9"/>
+      <c r="F969" s="7"/>
     </row>
     <row r="970">
-      <c r="F970" s="9"/>
+      <c r="F970" s="7"/>
     </row>
     <row r="971">
-      <c r="F971" s="9"/>
+      <c r="F971" s="7"/>
     </row>
     <row r="972">
-      <c r="F972" s="9"/>
+      <c r="F972" s="7"/>
     </row>
     <row r="973">
-      <c r="F973" s="9"/>
+      <c r="F973" s="7"/>
     </row>
     <row r="974">
-      <c r="F974" s="9"/>
+      <c r="F974" s="7"/>
     </row>
     <row r="975">
-      <c r="F975" s="9"/>
+      <c r="F975" s="7"/>
     </row>
     <row r="976">
-      <c r="F976" s="9"/>
+      <c r="F976" s="7"/>
     </row>
     <row r="977">
-      <c r="F977" s="9"/>
+      <c r="F977" s="7"/>
     </row>
     <row r="978">
-      <c r="F978" s="9"/>
+      <c r="F978" s="7"/>
     </row>
     <row r="979">
-      <c r="F979" s="9"/>
+      <c r="F979" s="7"/>
     </row>
     <row r="980">
-      <c r="F980" s="9"/>
+      <c r="F980" s="7"/>
     </row>
     <row r="981">
-      <c r="F981" s="9"/>
+      <c r="F981" s="7"/>
     </row>
     <row r="982">
-      <c r="F982" s="9"/>
+      <c r="F982" s="7"/>
     </row>
     <row r="983">
-      <c r="F983" s="9"/>
+      <c r="F983" s="7"/>
     </row>
     <row r="984">
-      <c r="F984" s="9"/>
+      <c r="F984" s="7"/>
     </row>
     <row r="985">
-      <c r="F985" s="9"/>
+      <c r="F985" s="7"/>
     </row>
     <row r="986">
-      <c r="F986" s="9"/>
+      <c r="F986" s="7"/>
     </row>
     <row r="987">
-      <c r="F987" s="9"/>
+      <c r="F987" s="7"/>
     </row>
     <row r="988">
-      <c r="F988" s="9"/>
+      <c r="F988" s="7"/>
     </row>
     <row r="989">
-      <c r="F989" s="9"/>
+      <c r="F989" s="7"/>
     </row>
     <row r="990">
-      <c r="F990" s="9"/>
+      <c r="F990" s="7"/>
     </row>
     <row r="991">
-      <c r="F991" s="9"/>
+      <c r="F991" s="7"/>
     </row>
     <row r="992">
-      <c r="F992" s="9"/>
+      <c r="F992" s="7"/>
     </row>
     <row r="993">
-      <c r="F993" s="9"/>
+      <c r="F993" s="7"/>
     </row>
     <row r="994">
-      <c r="F994" s="9"/>
+      <c r="F994" s="7"/>
     </row>
     <row r="995">
-      <c r="F995" s="9"/>
+      <c r="F995" s="7"/>
     </row>
     <row r="996">
-      <c r="F996" s="9"/>
+      <c r="F996" s="7"/>
     </row>
     <row r="997">
-      <c r="F997" s="9"/>
+      <c r="F997" s="7"/>
     </row>
     <row r="998">
-      <c r="F998" s="9"/>
+      <c r="F998" s="7"/>
     </row>
     <row r="999">
-      <c r="F999" s="9"/>
+      <c r="F999" s="7"/>
     </row>
     <row r="1000">
-      <c r="F1000" s="9"/>
+      <c r="F1000" s="7"/>
     </row>
     <row r="1001">
-      <c r="F1001" s="9"/>
+      <c r="F1001" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$2:$G$4"/>
+  <autoFilter ref="$A$2:$I$4"/>
   <customSheetViews>
-    <customSheetView guid="{AADD0144-9195-49E4-9822-F67AE472B802}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B936B0B1-DF02-40D5-BCB6-86CF286B23A4}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$7"/>
     </customSheetView>
-    <customSheetView guid="{DAF9E434-143D-4C2F-BD3A-F42958B886A7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4318B231-53B8-4726-82BD-03FDEDD286E4}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$3:$A$28"/>
     </customSheetView>
-    <customSheetView guid="{3557EC7E-8B9C-4DD1-84AC-D25832B36FAD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F420EFAA-E1E7-4C15-A18B-9F49B707E26E}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$4:$A$501"/>
+    </customSheetView>
+    <customSheetView guid="{1D7BF479-05B9-4152-9B2B-CFBDDFCD1068}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$2:$G$4"/>
+    </customSheetView>
+    <customSheetView guid="{AFAA05CB-82C0-46F8-B97B-1146D381C75C}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$2:$G$4"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>